<commit_message>
ok fix e build ok
</commit_message>
<xml_diff>
--- a/orario_settimanale.xlsx
+++ b/orario_settimanale.xlsx
@@ -527,24 +527,24 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
           <t>LEO</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
           <t>SIMEONE</t>
@@ -552,12 +552,12 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>DOCENTE4</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>MOTORIA</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -585,57 +585,57 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>LEO</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
-        </is>
-      </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
         </is>
       </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>PALMISANO</t>
         </is>
       </c>
     </row>
@@ -657,47 +657,47 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -719,42 +719,42 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
@@ -771,57 +771,57 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>DOCENTE4</t>
+          <t>DOCENTE1</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L6" s="1" t="inlineStr">
         <is>
           <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -833,52 +833,52 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>DOCENTE4</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
-        </is>
-      </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
           <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr"/>
@@ -891,24 +891,24 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
+          <t>CICCIMARRA</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
-        </is>
-      </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
           <t>SIMEONE</t>
@@ -926,12 +926,12 @@
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
           <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="J8" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -949,57 +949,57 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
+        <is>
           <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="I9" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="J9" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
         </is>
       </c>
     </row>
@@ -1011,14 +1011,14 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
           <t>SCHIAVONE</t>
@@ -1046,22 +1046,22 @@
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
         </is>
       </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1073,22 +1073,22 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="I11" s="2" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="J11" s="2" t="inlineStr">
@@ -1135,14 +1135,14 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
           <t>SABATELLI</t>
@@ -1155,37 +1155,37 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L12" s="2" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1197,14 +1197,14 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>SABATELLI</t>
@@ -1217,14 +1217,14 @@
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
+          <t>DOCENTE4</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G13" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
           <t>SAVINO</t>
@@ -1237,12 +1237,12 @@
       </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K13" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE3</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="L13" s="2" t="inlineStr"/>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>DOCENTE4</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -1270,12 +1270,12 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>DOCENTE4</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
@@ -1295,12 +1295,12 @@
       </c>
       <c r="J14" s="3" t="inlineStr">
         <is>
-          <t>DOCENTE3</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K14" s="3" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="L14" s="3" t="inlineStr"/>
@@ -1313,49 +1313,49 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
           <t>LEO</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J15" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
       <c r="K15" s="3" t="inlineStr">
         <is>
           <t>ZIZZI</t>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -1385,47 +1385,47 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E16" s="3" t="inlineStr">
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
         <is>
           <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
         </is>
       </c>
     </row>
@@ -1437,12 +1437,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>DOCENTE1</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -1452,42 +1452,42 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="H17" s="3" t="inlineStr">
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I17" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J17" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="K17" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L17" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
         </is>
       </c>
     </row>
@@ -1499,57 +1499,57 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>DOCENTE1</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
           <t>LEO</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
+      <c r="G18" s="3" t="inlineStr">
         <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G18" s="3" t="inlineStr">
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
         <is>
           <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H18" s="3" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I18" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J18" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="K18" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L18" s="3" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -1561,42 +1561,42 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H19" s="3" t="inlineStr">
+      <c r="I19" s="3" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I19" s="3" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
@@ -1634,37 +1634,37 @@
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="I20" s="4" t="inlineStr">
+        <is>
           <t>PEPE</t>
         </is>
       </c>
-      <c r="I20" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
       <c r="J20" s="4" t="inlineStr">
         <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K20" s="4" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
         </is>
       </c>
       <c r="L20" s="4" t="inlineStr"/>
@@ -1677,57 +1677,57 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
           <t>MARANGI</t>
         </is>
       </c>
-      <c r="G21" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H21" s="4" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I21" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="J21" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K21" s="4" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L21" s="4" t="inlineStr">
+        <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J21" s="4" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
-        </is>
-      </c>
-      <c r="L21" s="4" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
         </is>
       </c>
     </row>
@@ -1769,17 +1769,17 @@
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>MOTORIA</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
@@ -1801,14 +1801,14 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
           <t>SCHIAVONE</t>
@@ -1816,42 +1816,42 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I23" s="4" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J23" s="4" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K23" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L23" s="4" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G23" s="4" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H23" s="4" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
-        </is>
-      </c>
-      <c r="I23" s="4" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="J23" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L23" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
         </is>
       </c>
     </row>
@@ -1878,42 +1878,42 @@
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L24" s="4" t="inlineStr">
+        <is>
           <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="I24" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L24" s="4" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -1930,47 +1930,47 @@
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
           <t>DOCENTE4</t>
         </is>
       </c>
-      <c r="D25" s="4" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F25" s="4" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="H25" s="4" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I25" s="4" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I25" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE3</t>
+          <t>MOTORIA</t>
         </is>
       </c>
       <c r="L25" s="4" t="inlineStr"/>
@@ -1988,19 +1988,19 @@
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>DOCENTE4</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="inlineStr">
+        <is>
           <t>CICCIMARRA</t>
         </is>
       </c>
-      <c r="E26" s="5" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F26" s="5" t="inlineStr">
         <is>
           <t>SAVINO</t>
@@ -2008,27 +2008,27 @@
       </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H26" s="5" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="I26" s="5" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J26" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
           <t>LEO</t>
-        </is>
-      </c>
-      <c r="H26" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I26" s="5" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J26" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K26" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="L26" s="5" t="inlineStr"/>
@@ -2041,57 +2041,57 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C27" s="5" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H27" s="5" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
           <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="E27" s="5" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F27" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G27" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="H27" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K27" s="5" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="L27" s="5" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
@@ -2118,19 +2118,19 @@
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F28" s="5" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
           <t>MARANGI</t>
         </is>
       </c>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
           <t>PEPE</t>
@@ -2138,17 +2138,17 @@
       </c>
       <c r="I28" s="5" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>MOTORIA</t>
         </is>
       </c>
       <c r="J28" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K28" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE3</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L28" s="5" t="inlineStr">
@@ -2165,22 +2165,22 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F29" s="5" t="inlineStr">
@@ -2195,12 +2195,12 @@
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
           <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="I29" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J29" s="5" t="inlineStr">
@@ -2232,19 +2232,19 @@
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
+          <t>CICCIMARRA</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E30" s="5" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F30" s="5" t="inlineStr">
         <is>
           <t>MARANGI</t>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE4</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="H30" s="5" t="inlineStr">
@@ -2262,12 +2262,12 @@
       </c>
       <c r="I30" s="5" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J30" s="5" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K30" s="5" t="inlineStr">
@@ -2411,62 +2411,62 @@
           <t>LUN1</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr"/>
-      <c r="C2" s="1" t="inlineStr"/>
-      <c r="D2" s="1" t="inlineStr"/>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr"/>
+      <c r="G2" s="1" t="inlineStr"/>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr"/>
+      <c r="M2" s="1" t="inlineStr"/>
+      <c r="N2" s="1" t="inlineStr"/>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr"/>
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr"/>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr"/>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2476,61 +2476,61 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr"/>
-      <c r="D3" s="1" t="inlineStr"/>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr"/>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
         <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr"/>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr"/>
-      <c r="M3" s="1" t="inlineStr">
+      <c r="M3" s="1" t="inlineStr"/>
+      <c r="N3" s="1" t="inlineStr"/>
+      <c r="O3" s="1" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="N3" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="O3" s="1" t="inlineStr">
+      <c r="P3" s="1" t="inlineStr">
         <is>
           <t>3A</t>
-        </is>
-      </c>
-      <c r="P3" s="1" t="inlineStr">
-        <is>
-          <t>1A</t>
         </is>
       </c>
       <c r="Q3" s="1" t="inlineStr"/>
@@ -2551,17 +2551,21 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="D4" s="1" t="inlineStr"/>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
           <t>3A</t>
@@ -2572,32 +2576,28 @@
           <t>3B</t>
         </is>
       </c>
-      <c r="I4" s="1" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr"/>
+      <c r="J4" s="1" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="J4" s="1" t="inlineStr"/>
       <c r="K4" s="1" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
+      <c r="L4" s="1" t="inlineStr"/>
       <c r="M4" s="1" t="inlineStr"/>
       <c r="N4" s="1" t="inlineStr"/>
       <c r="O4" s="1" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="P4" s="1" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="Q4" s="1" t="inlineStr"/>
@@ -2618,8 +2618,16 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr"/>
-      <c r="E5" s="1" t="inlineStr"/>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
           <t>2B</t>
@@ -2627,27 +2635,19 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
           <t>3A</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr"/>
+      <c r="I5" s="1" t="inlineStr"/>
+      <c r="J5" s="1" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
@@ -2659,12 +2659,12 @@
       <c r="N5" s="1" t="inlineStr"/>
       <c r="O5" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="P5" s="1" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="Q5" s="1" t="inlineStr"/>
@@ -2675,66 +2675,66 @@
           <t>LUN5</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr"/>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr"/>
+      <c r="I6" s="1" t="inlineStr"/>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr"/>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="inlineStr">
+      <c r="L6" s="1" t="inlineStr">
         <is>
           <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
         </is>
       </c>
       <c r="M6" s="1" t="inlineStr"/>
       <c r="N6" s="1" t="inlineStr"/>
-      <c r="O6" s="1" t="inlineStr"/>
+      <c r="O6" s="1" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
       <c r="P6" s="1" t="inlineStr">
         <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="Q6" s="1" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="Q6" s="1" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2742,62 +2742,62 @@
           <t>LUN6</t>
         </is>
       </c>
-      <c r="B7" s="1" t="inlineStr"/>
-      <c r="C7" s="1" t="inlineStr"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr"/>
+      <c r="I7" s="1" t="inlineStr"/>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L7" s="1" t="inlineStr"/>
+      <c r="M7" s="1" t="inlineStr"/>
+      <c r="N7" s="1" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="O7" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="P7" s="1" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L7" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="M7" s="1" t="inlineStr"/>
-      <c r="N7" s="1" t="inlineStr"/>
-      <c r="O7" s="1" t="inlineStr"/>
-      <c r="P7" s="1" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="Q7" s="1" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="Q7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -2807,18 +2807,18 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr"/>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="D8" s="2" t="inlineStr"/>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr"/>
@@ -2832,7 +2832,11 @@
           <t>3A</t>
         </is>
       </c>
-      <c r="I8" s="2" t="inlineStr"/>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
       <c r="J8" s="2" t="inlineStr"/>
       <c r="K8" s="2" t="inlineStr">
         <is>
@@ -2841,7 +2845,7 @@
       </c>
       <c r="L8" s="2" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="M8" s="2" t="inlineStr">
@@ -2851,14 +2855,10 @@
       </c>
       <c r="N8" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O8" s="2" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="O8" s="2" t="inlineStr"/>
       <c r="P8" s="2" t="inlineStr"/>
       <c r="Q8" s="2" t="inlineStr"/>
     </row>
@@ -2870,27 +2870,23 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="D9" s="2" t="inlineStr"/>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
@@ -2903,7 +2899,11 @@
           <t>3A</t>
         </is>
       </c>
-      <c r="I9" s="2" t="inlineStr"/>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="J9" s="2" t="inlineStr"/>
       <c r="K9" s="2" t="inlineStr">
         <is>
@@ -2912,20 +2912,20 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="M9" s="2" t="inlineStr"/>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="M9" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
       <c r="N9" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O9" s="2" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="O9" s="2" t="inlineStr"/>
       <c r="P9" s="2" t="inlineStr"/>
       <c r="Q9" s="2" t="inlineStr"/>
     </row>
@@ -2937,62 +2937,62 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr"/>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I10" s="2" t="inlineStr"/>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
+      <c r="L10" s="2" t="inlineStr"/>
+      <c r="M10" s="2" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="inlineStr"/>
-      <c r="N10" s="2" t="inlineStr"/>
-      <c r="O10" s="2" t="inlineStr">
+      <c r="N10" s="2" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
+      <c r="O10" s="2" t="inlineStr"/>
       <c r="P10" s="2" t="inlineStr"/>
       <c r="Q10" s="2" t="inlineStr"/>
     </row>
@@ -3004,14 +3004,14 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
@@ -3037,11 +3037,7 @@
           <t>3B</t>
         </is>
       </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
+      <c r="I11" s="2" t="inlineStr"/>
       <c r="J11" s="2" t="inlineStr">
         <is>
           <t>4A</t>
@@ -3054,13 +3050,17 @@
       </c>
       <c r="L11" s="2" t="inlineStr"/>
       <c r="M11" s="2" t="inlineStr"/>
-      <c r="N11" s="2" t="inlineStr"/>
-      <c r="O11" s="2" t="inlineStr"/>
-      <c r="P11" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
+      <c r="N11" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="O11" s="2" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="P11" s="2" t="inlineStr"/>
       <c r="Q11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
@@ -3071,63 +3071,63 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="inlineStr"/>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
           <t>5B</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I12" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
         </is>
       </c>
       <c r="L12" s="2" t="inlineStr"/>
       <c r="M12" s="2" t="inlineStr"/>
-      <c r="N12" s="2" t="inlineStr"/>
-      <c r="O12" s="2" t="inlineStr"/>
-      <c r="P12" s="2" t="inlineStr">
+      <c r="N12" s="2" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
+      <c r="O12" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="P12" s="2" t="inlineStr"/>
       <c r="Q12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
@@ -3136,19 +3136,15 @@
           <t>MAR6</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr"/>
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
@@ -3161,14 +3157,10 @@
           <t>2B</t>
         </is>
       </c>
-      <c r="G13" s="2" t="inlineStr">
+      <c r="G13" s="2" t="inlineStr"/>
+      <c r="H13" s="2" t="inlineStr">
         <is>
           <t>3B</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="inlineStr">
-        <is>
-          <t>3A</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
@@ -3177,21 +3169,29 @@
           <t>4B</t>
         </is>
       </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="K13" s="2" t="inlineStr"/>
       <c r="L13" s="2" t="inlineStr"/>
       <c r="M13" s="2" t="inlineStr"/>
-      <c r="N13" s="2" t="inlineStr"/>
-      <c r="O13" s="2" t="inlineStr"/>
+      <c r="N13" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="Q13" s="2" t="inlineStr"/>
+      <c r="Q13" s="2" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -3204,26 +3204,14 @@
           <t>1B</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="C14" s="3" t="inlineStr"/>
+      <c r="D14" s="3" t="inlineStr"/>
       <c r="E14" s="3" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
+      <c r="F14" s="3" t="inlineStr"/>
       <c r="G14" s="3" t="inlineStr"/>
       <c r="H14" s="3" t="inlineStr">
         <is>
@@ -3242,17 +3230,29 @@
       </c>
       <c r="K14" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L14" s="3" t="inlineStr"/>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="M14" s="3" t="inlineStr"/>
       <c r="N14" s="3" t="inlineStr"/>
-      <c r="O14" s="3" t="inlineStr"/>
-      <c r="P14" s="3" t="inlineStr"/>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="P14" s="3" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
       <c r="Q14" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
@@ -3264,61 +3264,61 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="C15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="3" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr"/>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J15" s="3" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K15" s="3" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L15" s="3" t="inlineStr"/>
       <c r="M15" s="3" t="inlineStr"/>
       <c r="N15" s="3" t="inlineStr"/>
       <c r="O15" s="3" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="P15" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="Q15" s="3" t="inlineStr"/>
@@ -3341,51 +3341,51 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr"/>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="K16" s="3" t="inlineStr"/>
       <c r="L16" s="3" t="inlineStr"/>
       <c r="M16" s="3" t="inlineStr"/>
       <c r="N16" s="3" t="inlineStr"/>
       <c r="O16" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="Q16" s="3" t="inlineStr"/>
@@ -3396,22 +3396,22 @@
           <t>MER4</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr"/>
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E17" s="3" t="inlineStr"/>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
           <t>2A</t>
@@ -3419,22 +3419,22 @@
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="H17" s="3" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I17" s="3" t="inlineStr">
+      <c r="J17" s="3" t="inlineStr">
         <is>
           <t>4A</t>
-        </is>
-      </c>
-      <c r="J17" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
         </is>
       </c>
       <c r="K17" s="3" t="inlineStr"/>
@@ -3447,12 +3447,12 @@
       </c>
       <c r="O17" s="3" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="P17" s="3" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="Q17" s="3" t="inlineStr"/>
@@ -3463,18 +3463,22 @@
           <t>MER5</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" s="3" t="inlineStr"/>
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr"/>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr"/>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
           <t>2A</t>
@@ -3482,44 +3486,40 @@
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="H18" s="3" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J18" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
       <c r="K18" s="3" t="inlineStr"/>
-      <c r="L18" s="3" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
+      <c r="L18" s="3" t="inlineStr"/>
       <c r="M18" s="3" t="inlineStr"/>
       <c r="N18" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="O18" s="3" t="inlineStr">
         <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="P18" s="3" t="inlineStr">
+        <is>
           <t>1B</t>
-        </is>
-      </c>
-      <c r="P18" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
         </is>
       </c>
       <c r="Q18" s="3" t="inlineStr"/>
@@ -3530,21 +3530,25 @@
           <t>MER6</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr"/>
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr"/>
       <c r="D19" s="3" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="E19" s="3" t="inlineStr"/>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
@@ -3559,30 +3563,26 @@
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr"/>
       <c r="K19" s="3" t="inlineStr"/>
-      <c r="L19" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="M19" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
+      <c r="L19" s="3" t="inlineStr"/>
+      <c r="M19" s="3" t="inlineStr"/>
       <c r="N19" s="3" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="O19" s="3" t="inlineStr"/>
+      <c r="O19" s="3" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="P19" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="Q19" s="3" t="inlineStr"/>
@@ -3593,61 +3593,61 @@
           <t>GIO1</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr"/>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="D20" s="4" t="inlineStr"/>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="F20" s="4" t="inlineStr"/>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H20" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I20" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J20" s="4" t="inlineStr"/>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L20" s="4" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr"/>
-      <c r="H20" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I20" s="4" t="inlineStr">
+      <c r="M20" s="4" t="inlineStr"/>
+      <c r="N20" s="4" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J20" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K20" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L20" s="4" t="inlineStr"/>
-      <c r="M20" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="N20" s="4" t="inlineStr"/>
-      <c r="O20" s="4" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="P20" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
+      <c r="O20" s="4" t="inlineStr"/>
+      <c r="P20" s="4" t="inlineStr"/>
       <c r="Q20" s="4" t="inlineStr"/>
     </row>
     <row r="21">
@@ -3656,65 +3656,65 @@
           <t>GIO2</t>
         </is>
       </c>
-      <c r="B21" s="4" t="inlineStr"/>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="inlineStr"/>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H21" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I21" s="4" t="inlineStr">
+        <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G21" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H21" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
+      <c r="J21" s="4" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J21" s="4" t="inlineStr">
+      <c r="K21" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L21" s="4" t="inlineStr"/>
+      <c r="M21" s="4" t="inlineStr"/>
+      <c r="N21" s="4" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L21" s="4" t="inlineStr"/>
-      <c r="M21" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="N21" s="4" t="inlineStr"/>
-      <c r="O21" s="4" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="P21" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="O21" s="4" t="inlineStr"/>
+      <c r="P21" s="4" t="inlineStr"/>
       <c r="Q21" s="4" t="inlineStr"/>
     </row>
     <row r="22">
@@ -3733,7 +3733,11 @@
           <t>1B</t>
         </is>
       </c>
-      <c r="D22" s="4" t="inlineStr"/>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
           <t>2B</t>
@@ -3761,27 +3765,23 @@
       </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr"/>
+      <c r="M22" s="4" t="inlineStr"/>
+      <c r="N22" s="4" t="inlineStr"/>
+      <c r="O22" s="4" t="inlineStr"/>
+      <c r="P22" s="4" t="inlineStr">
+        <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr"/>
-      <c r="M22" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="N22" s="4" t="inlineStr"/>
-      <c r="O22" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="P22" s="4" t="inlineStr"/>
       <c r="Q22" s="4" t="inlineStr"/>
     </row>
     <row r="23">
@@ -3792,63 +3792,63 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I23" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J23" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K23" s="4" t="inlineStr">
+        <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr">
+      <c r="L23" s="4" t="inlineStr"/>
+      <c r="M23" s="4" t="inlineStr"/>
+      <c r="N23" s="4" t="inlineStr"/>
+      <c r="O23" s="4" t="inlineStr"/>
+      <c r="P23" s="4" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G23" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H23" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I23" s="4" t="inlineStr"/>
-      <c r="J23" s="4" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L23" s="4" t="inlineStr"/>
-      <c r="M23" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="N23" s="4" t="inlineStr"/>
-      <c r="O23" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="P23" s="4" t="inlineStr"/>
       <c r="Q23" s="4" t="inlineStr"/>
     </row>
     <row r="24">
@@ -3872,50 +3872,50 @@
           <t>5B</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
+      <c r="E24" s="4" t="inlineStr"/>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr"/>
+      <c r="L24" s="4" t="inlineStr"/>
+      <c r="M24" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="N24" s="4" t="inlineStr"/>
+      <c r="O24" s="4" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr">
+      <c r="P24" s="4" t="inlineStr">
         <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="I24" s="4" t="inlineStr"/>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L24" s="4" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M24" s="4" t="inlineStr"/>
-      <c r="N24" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O24" s="4" t="inlineStr"/>
-      <c r="P24" s="4" t="inlineStr"/>
       <c r="Q24" s="4" t="inlineStr"/>
     </row>
     <row r="25">
@@ -3924,7 +3924,11 @@
           <t>GIO6</t>
         </is>
       </c>
-      <c r="B25" s="4" t="inlineStr"/>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
           <t>1A</t>
@@ -3932,52 +3936,48 @@
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="inlineStr"/>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr"/>
+      <c r="H25" s="4" t="inlineStr"/>
+      <c r="I25" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J25" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K25" s="4" t="inlineStr"/>
+      <c r="L25" s="4" t="inlineStr"/>
+      <c r="M25" s="4" t="inlineStr">
+        <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E25" s="4" t="inlineStr">
+      <c r="N25" s="4" t="inlineStr"/>
+      <c r="O25" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="P25" s="4" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F25" s="4" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G25" s="4" t="inlineStr">
+      <c r="Q25" s="4" t="inlineStr">
         <is>
           <t>3A</t>
-        </is>
-      </c>
-      <c r="H25" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I25" s="4" t="inlineStr"/>
-      <c r="J25" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K25" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L25" s="4" t="inlineStr"/>
-      <c r="M25" s="4" t="inlineStr"/>
-      <c r="N25" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O25" s="4" t="inlineStr"/>
-      <c r="P25" s="4" t="inlineStr"/>
-      <c r="Q25" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
         </is>
       </c>
     </row>
@@ -3987,62 +3987,62 @@
           <t>VEN1</t>
         </is>
       </c>
-      <c r="B26" s="5" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="B26" s="5" t="inlineStr"/>
       <c r="C26" s="5" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="D26" s="5" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="D26" s="5" t="inlineStr"/>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="F26" s="5" t="inlineStr"/>
       <c r="G26" s="5" t="inlineStr"/>
-      <c r="H26" s="5" t="inlineStr"/>
+      <c r="H26" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="J26" s="5" t="inlineStr">
+      <c r="J26" s="5" t="inlineStr"/>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L26" s="5" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="M26" s="5" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="K26" s="5" t="inlineStr"/>
-      <c r="L26" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="M26" s="5" t="inlineStr"/>
-      <c r="N26" s="5" t="inlineStr">
+      <c r="N26" s="5" t="inlineStr"/>
+      <c r="O26" s="5" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="O26" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
       <c r="P26" s="5" t="inlineStr">
         <is>
           <t>3A</t>
         </is>
       </c>
-      <c r="Q26" s="5" t="inlineStr"/>
+      <c r="Q26" s="5" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
@@ -4050,63 +4050,63 @@
           <t>VEN2</t>
         </is>
       </c>
-      <c r="B27" s="5" t="inlineStr">
+      <c r="B27" s="5" t="inlineStr"/>
+      <c r="C27" s="5" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C27" s="5" t="inlineStr">
+      <c r="D27" s="5" t="inlineStr"/>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H27" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr"/>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="M27" s="5" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="N27" s="5" t="inlineStr"/>
+      <c r="O27" s="5" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="D27" s="5" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="E27" s="5" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="F27" s="5" t="inlineStr"/>
-      <c r="G27" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H27" s="5" t="inlineStr"/>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K27" s="5" t="inlineStr"/>
-      <c r="L27" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="M27" s="5" t="inlineStr"/>
-      <c r="N27" s="5" t="inlineStr">
+      <c r="P27" s="5" t="inlineStr">
         <is>
           <t>4B</t>
-        </is>
-      </c>
-      <c r="O27" s="5" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="P27" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
         </is>
       </c>
       <c r="Q27" s="5" t="inlineStr"/>
@@ -4122,58 +4122,58 @@
           <t>1B</t>
         </is>
       </c>
-      <c r="C28" s="5" t="inlineStr">
+      <c r="C28" s="5" t="inlineStr"/>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr"/>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H28" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I28" s="5" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J28" s="5" t="inlineStr"/>
+      <c r="K28" s="5" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L28" s="5" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="M28" s="5" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="N28" s="5" t="inlineStr"/>
+      <c r="O28" s="5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="P28" s="5" t="inlineStr">
         <is>
           <t>1A</t>
-        </is>
-      </c>
-      <c r="D28" s="5" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="E28" s="5" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="F28" s="5" t="inlineStr"/>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H28" s="5" t="inlineStr"/>
-      <c r="I28" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="J28" s="5" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K28" s="5" t="inlineStr"/>
-      <c r="L28" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M28" s="5" t="inlineStr"/>
-      <c r="N28" s="5" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="O28" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="P28" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
         </is>
       </c>
       <c r="Q28" s="5" t="inlineStr"/>
@@ -4186,25 +4186,21 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="C29" s="5" t="inlineStr">
-        <is>
           <t>1A</t>
         </is>
       </c>
+      <c r="C29" s="5" t="inlineStr"/>
       <c r="D29" s="5" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E29" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="F29" s="5" t="inlineStr"/>
+      <c r="E29" s="5" t="inlineStr"/>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
           <t>3A</t>
@@ -4218,7 +4214,7 @@
       </c>
       <c r="J29" s="5" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="K29" s="5" t="inlineStr">
@@ -4226,16 +4222,20 @@
           <t>5A</t>
         </is>
       </c>
-      <c r="L29" s="5" t="inlineStr"/>
+      <c r="L29" s="5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
       <c r="M29" s="5" t="inlineStr"/>
       <c r="N29" s="5" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="O29" s="5" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="P29" s="5" t="inlineStr">
@@ -4256,24 +4256,16 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="C30" s="5" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="C30" s="5" t="inlineStr"/>
       <c r="D30" s="5" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E30" s="5" t="inlineStr">
+      <c r="E30" s="5" t="inlineStr"/>
+      <c r="F30" s="5" t="inlineStr">
         <is>
           <t>2B</t>
-        </is>
-      </c>
-      <c r="F30" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
         </is>
       </c>
       <c r="G30" s="5" t="inlineStr">
@@ -4287,9 +4279,21 @@
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="J30" s="5" t="inlineStr"/>
-      <c r="K30" s="5" t="inlineStr"/>
-      <c r="L30" s="5" t="inlineStr"/>
+      <c r="J30" s="5" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K30" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L30" s="5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
       <c r="M30" s="5" t="inlineStr"/>
       <c r="N30" s="5" t="inlineStr">
         <is>
@@ -4298,19 +4302,15 @@
       </c>
       <c r="O30" s="5" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="P30" s="5" t="inlineStr">
         <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="Q30" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="Q30" s="5" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="inlineStr">

</xml_diff>

<commit_message>
aggiunto vincolo specifico Minimo 2 ore/giorno se presente
</commit_message>
<xml_diff>
--- a/orario_settimanale.xlsx
+++ b/orario_settimanale.xlsx
@@ -537,27 +537,27 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>CICCIMARRA</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
           <t>LEO</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>DOCENTE4</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
@@ -585,44 +585,44 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
           <t>DOCENTE3</t>
@@ -635,7 +635,7 @@
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -657,27 +657,27 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
           <t>MARANGI</t>
         </is>
       </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="I4" s="1" t="inlineStr">
@@ -687,17 +687,17 @@
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
         </is>
       </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -729,22 +729,22 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
           <t>MARANGI</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
@@ -781,32 +781,32 @@
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
@@ -833,22 +833,22 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
@@ -858,17 +858,17 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
           <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -911,27 +911,27 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>DOCENTE4</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>MOTORIA</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -959,37 +959,37 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
           <t>PEPE</t>
         </is>
       </c>
-      <c r="I9" s="2" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
-        </is>
-      </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K9" s="2" t="inlineStr">
@@ -999,7 +999,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>PALMISANO</t>
         </is>
       </c>
     </row>
@@ -1011,34 +1011,34 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
           <t>MARANGI</t>
         </is>
       </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
           <t>PALMISANO</t>
@@ -1046,12 +1046,12 @@
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>MOTORIA</t>
+          <t>DOCENTE3</t>
         </is>
       </c>
       <c r="K10" s="2" t="inlineStr">
@@ -1088,27 +1088,27 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
           <t>LEO</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="J11" s="2" t="inlineStr">
@@ -1145,47 +1145,47 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr">
+        <is>
           <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="I12" s="2" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L12" s="2" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
         </is>
       </c>
     </row>
@@ -1202,22 +1202,22 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE4</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr">
@@ -1237,12 +1237,12 @@
       </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE3</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K13" s="2" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>MOTORIA</t>
         </is>
       </c>
       <c r="L13" s="2" t="inlineStr"/>
@@ -1255,14 +1255,14 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
           <t>DOCENTE4</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
           <t>SABATELLI</t>
@@ -1270,37 +1270,37 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>DOCENTE2</t>
         </is>
       </c>
       <c r="J14" s="3" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>LEO</t>
         </is>
       </c>
       <c r="L14" s="3" t="inlineStr"/>
@@ -1313,24 +1313,24 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
           <t>MARANGI</t>
@@ -1343,27 +1343,27 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J15" s="3" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="K15" s="3" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L15" s="3" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -1375,57 +1375,57 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
+      <c r="I16" s="3" t="inlineStr">
         <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I16" s="3" t="inlineStr">
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
         </is>
       </c>
     </row>
@@ -1442,17 +1442,17 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
@@ -1499,32 +1499,32 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
           <t>DOCENTE1</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
@@ -1539,17 +1539,17 @@
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
           <t>DOCENTE3</t>
         </is>
       </c>
-      <c r="K18" s="3" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
       <c r="L18" s="3" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1571,27 +1571,27 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
           <t>MARANGI</t>
         </is>
       </c>
-      <c r="G19" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>DOCENTE4</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
@@ -1644,22 +1644,22 @@
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE2</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE3</t>
+          <t>MOTORIA</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
@@ -1687,14 +1687,14 @@
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
+          <t>CICCIMARRA</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
           <t>SIMEONE</t>
@@ -1702,32 +1702,32 @@
       </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="H21" s="4" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I21" s="4" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="J21" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K21" s="4" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L21" s="4" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="J21" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L21" s="4" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1739,57 +1739,57 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G22" s="4" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H22" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1801,22 +1801,22 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
         </is>
       </c>
       <c r="F23" s="4" t="inlineStr">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
@@ -1878,42 +1878,42 @@
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
           <t>LEO</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr">
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="L24" s="4" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I24" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L24" s="4" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE1</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -1935,42 +1935,42 @@
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="F25" s="4" t="inlineStr">
         <is>
-          <t>DOCENTE4</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="H25" s="4" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I25" s="4" t="inlineStr">
+        <is>
           <t>PEPE</t>
         </is>
       </c>
-      <c r="I25" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
       <c r="J25" s="4" t="inlineStr">
         <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K25" s="4" t="inlineStr">
+        <is>
           <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="K25" s="4" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
         </is>
       </c>
       <c r="L25" s="4" t="inlineStr"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>DOCENTE4</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
@@ -1998,37 +1998,37 @@
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F26" s="5" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="G26" s="5" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I26" s="5" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J26" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
           <t>MOTORIA</t>
-        </is>
-      </c>
-      <c r="I26" s="5" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J26" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K26" s="5" t="inlineStr">
-        <is>
-          <t>LEO</t>
         </is>
       </c>
       <c r="L26" s="5" t="inlineStr"/>
@@ -2041,57 +2041,57 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H27" s="5" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
           <t>LEO</t>
         </is>
       </c>
-      <c r="C27" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE1</t>
-        </is>
-      </c>
-      <c r="D27" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E27" s="5" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F27" s="5" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G27" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H27" s="5" t="inlineStr">
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K27" s="5" t="inlineStr">
-        <is>
-          <t>MOTORIA</t>
-        </is>
-      </c>
-      <c r="L27" s="5" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
         </is>
       </c>
     </row>
@@ -2103,57 +2103,57 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>DOCENTE1</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H28" s="5" t="inlineStr">
+        <is>
           <t>SAVINO</t>
         </is>
       </c>
-      <c r="C28" s="5" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
-      <c r="D28" s="5" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="E28" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F28" s="5" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H28" s="5" t="inlineStr">
+      <c r="I28" s="5" t="inlineStr">
         <is>
           <t>PEPE</t>
         </is>
       </c>
-      <c r="I28" s="5" t="inlineStr">
+      <c r="J28" s="5" t="inlineStr">
         <is>
           <t>MOTORIA</t>
         </is>
       </c>
-      <c r="J28" s="5" t="inlineStr">
+      <c r="K28" s="5" t="inlineStr">
         <is>
           <t>DOCENTE3</t>
         </is>
       </c>
-      <c r="K28" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
       <c r="L28" s="5" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>SABATELLI</t>
         </is>
       </c>
     </row>
@@ -2165,57 +2165,57 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DOCENTE1</t>
         </is>
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t>SAVINO</t>
+        </is>
+      </c>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H29" s="5" t="inlineStr">
+        <is>
+          <t>MOTORIA</t>
+        </is>
+      </c>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J29" s="5" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K29" s="5" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="L29" s="5" t="inlineStr">
+        <is>
           <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="E29" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F29" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G29" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO</t>
-        </is>
-      </c>
-      <c r="H29" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I29" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="J29" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K29" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L29" s="5" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -2227,57 +2227,57 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>SAVINO</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
-          <t>SAVINO</t>
+          <t>DOCENTE1</t>
         </is>
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
           <t>CICCIMARRA</t>
         </is>
       </c>
-      <c r="E30" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F30" s="5" t="inlineStr">
         <is>
+          <t>DOCENTE4</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H30" s="5" t="inlineStr">
+        <is>
+          <t>DOCENTE2</t>
+        </is>
+      </c>
+      <c r="I30" s="5" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J30" s="5" t="inlineStr">
+        <is>
+          <t>DOCENTE3</t>
+        </is>
+      </c>
+      <c r="K30" s="5" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="L30" s="5" t="inlineStr">
+        <is>
           <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G30" s="5" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="H30" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE2</t>
-        </is>
-      </c>
-      <c r="I30" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J30" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K30" s="5" t="inlineStr">
-        <is>
-          <t>DOCENTE3</t>
-        </is>
-      </c>
-      <c r="L30" s="5" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -2426,47 +2426,47 @@
           <t>5A</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr"/>
+      <c r="F2" s="1" t="inlineStr"/>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr"/>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr"/>
-      <c r="G2" s="1" t="inlineStr"/>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr"/>
       <c r="M2" s="1" t="inlineStr"/>
       <c r="N2" s="1" t="inlineStr"/>
       <c r="O2" s="1" t="inlineStr">
         <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr"/>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
+      <c r="Q2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2476,30 +2476,30 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr"/>
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr"/>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
           <t>3B</t>
@@ -2510,27 +2510,27 @@
           <t>4A</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr">
+      <c r="J3" s="1" t="inlineStr"/>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
         <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr"/>
       <c r="M3" s="1" t="inlineStr"/>
       <c r="N3" s="1" t="inlineStr"/>
       <c r="O3" s="1" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
           <t>4B</t>
-        </is>
-      </c>
-      <c r="P3" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
         </is>
       </c>
       <c r="Q3" s="1" t="inlineStr"/>
@@ -2553,27 +2553,23 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
           <t>3A</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
         </is>
       </c>
       <c r="I4" s="1" t="inlineStr"/>
@@ -2584,22 +2580,26 @@
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr"/>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
       <c r="M4" s="1" t="inlineStr"/>
-      <c r="N4" s="1" t="inlineStr"/>
+      <c r="N4" s="1" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="O4" s="1" t="inlineStr">
         <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="P4" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="P4" s="1" t="inlineStr"/>
       <c r="Q4" s="1" t="inlineStr"/>
     </row>
     <row r="5">
@@ -2635,38 +2635,38 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
           <t>3A</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr"/>
       <c r="I5" s="1" t="inlineStr"/>
       <c r="J5" s="1" t="inlineStr">
         <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="M5" s="1" t="inlineStr"/>
+      <c r="N5" s="1" t="inlineStr">
+        <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M5" s="1" t="inlineStr"/>
-      <c r="N5" s="1" t="inlineStr"/>
-      <c r="O5" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="P5" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
+      <c r="O5" s="1" t="inlineStr"/>
+      <c r="P5" s="1" t="inlineStr"/>
       <c r="Q5" s="1" t="inlineStr"/>
     </row>
     <row r="6">
@@ -2692,48 +2692,48 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr"/>
       <c r="I6" s="1" t="inlineStr"/>
       <c r="J6" s="1" t="inlineStr">
         <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L6" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="M6" s="1" t="inlineStr"/>
+      <c r="N6" s="1" t="inlineStr">
+        <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M6" s="1" t="inlineStr"/>
-      <c r="N6" s="1" t="inlineStr"/>
-      <c r="O6" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="P6" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
+      <c r="O6" s="1" t="inlineStr"/>
+      <c r="P6" s="1" t="inlineStr"/>
       <c r="Q6" s="1" t="inlineStr"/>
     </row>
     <row r="7">
@@ -2744,23 +2744,27 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E7" s="1" t="inlineStr"/>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
@@ -2768,11 +2772,15 @@
           <t>3A</t>
         </is>
       </c>
-      <c r="H7" s="1" t="inlineStr"/>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
       <c r="I7" s="1" t="inlineStr"/>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
@@ -2784,19 +2792,11 @@
       <c r="M7" s="1" t="inlineStr"/>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O7" s="1" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="P7" s="1" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="O7" s="1" t="inlineStr"/>
+      <c r="P7" s="1" t="inlineStr"/>
       <c r="Q7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
@@ -2805,17 +2805,17 @@
           <t>MAR1</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="B8" s="2" t="inlineStr"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>2B</t>
@@ -2824,17 +2824,13 @@
       <c r="F8" s="2" t="inlineStr"/>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
           <t>3A</t>
         </is>
       </c>
+      <c r="H8" s="2" t="inlineStr"/>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr"/>
@@ -2848,19 +2844,23 @@
           <t>2A</t>
         </is>
       </c>
-      <c r="M8" s="2" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="N8" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="O8" s="2" t="inlineStr"/>
-      <c r="P8" s="2" t="inlineStr"/>
-      <c r="Q8" s="2" t="inlineStr"/>
+      <c r="M8" s="2" t="inlineStr"/>
+      <c r="N8" s="2" t="inlineStr"/>
+      <c r="O8" s="2" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="P8" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="Q8" s="2" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -2878,55 +2878,55 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr"/>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr"/>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr"/>
+      <c r="M9" s="2" t="inlineStr"/>
+      <c r="N9" s="2" t="inlineStr"/>
+      <c r="O9" s="2" t="inlineStr">
+        <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I9" s="2" t="inlineStr">
+      <c r="P9" s="2" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J9" s="2" t="inlineStr"/>
-      <c r="K9" s="2" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M9" s="2" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="N9" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="O9" s="2" t="inlineStr"/>
-      <c r="P9" s="2" t="inlineStr"/>
       <c r="Q9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
@@ -2937,63 +2937,63 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr"/>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr"/>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr"/>
+      <c r="M10" s="2" t="inlineStr"/>
+      <c r="N10" s="2" t="inlineStr"/>
+      <c r="O10" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="P10" s="2" t="inlineStr">
+        <is>
           <t>3A</t>
         </is>
       </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I10" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr"/>
-      <c r="M10" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="N10" s="2" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O10" s="2" t="inlineStr"/>
-      <c r="P10" s="2" t="inlineStr"/>
       <c r="Q10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
@@ -3029,12 +3029,12 @@
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
           <t>3A</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>3B</t>
         </is>
       </c>
       <c r="I11" s="2" t="inlineStr"/>
@@ -3050,17 +3050,17 @@
       </c>
       <c r="L11" s="2" t="inlineStr"/>
       <c r="M11" s="2" t="inlineStr"/>
-      <c r="N11" s="2" t="inlineStr">
+      <c r="N11" s="2" t="inlineStr"/>
+      <c r="O11" s="2" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="O11" s="2" t="inlineStr">
+      <c r="P11" s="2" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="P11" s="2" t="inlineStr"/>
       <c r="Q11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
@@ -3079,24 +3079,20 @@
           <t>1B</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="D12" s="2" t="inlineStr"/>
       <c r="E12" s="2" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
@@ -3107,24 +3103,28 @@
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr"/>
+      <c r="M12" s="2" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="N12" s="2" t="inlineStr">
+        <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="L12" s="2" t="inlineStr"/>
-      <c r="M12" s="2" t="inlineStr"/>
-      <c r="N12" s="2" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
       <c r="O12" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="P12" s="2" t="inlineStr"/>
@@ -3136,28 +3136,28 @@
           <t>MAR6</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr"/>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="C13" s="2" t="inlineStr"/>
+      <c r="D13" s="2" t="inlineStr"/>
       <c r="E13" s="2" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G13" s="2" t="inlineStr"/>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
           <t>3B</t>
@@ -3169,12 +3169,20 @@
           <t>4B</t>
         </is>
       </c>
-      <c r="K13" s="2" t="inlineStr"/>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="L13" s="2" t="inlineStr"/>
-      <c r="M13" s="2" t="inlineStr"/>
+      <c r="M13" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
       <c r="N13" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="O13" s="2" t="inlineStr">
@@ -3182,16 +3190,8 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="P13" s="2" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="Q13" s="2" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
+      <c r="P13" s="2" t="inlineStr"/>
+      <c r="Q13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr"/>
@@ -3211,48 +3211,48 @@
           <t>2A</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr"/>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="G14" s="3" t="inlineStr"/>
       <c r="H14" s="3" t="inlineStr">
         <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr"/>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr"/>
+      <c r="M14" s="3" t="inlineStr"/>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="P14" s="3" t="inlineStr">
+        <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J14" s="3" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L14" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="M14" s="3" t="inlineStr"/>
-      <c r="N14" s="3" t="inlineStr"/>
-      <c r="O14" s="3" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="P14" s="3" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
       <c r="Q14" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
     </row>
@@ -3264,21 +3264,21 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr"/>
       <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="3" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
           <t>3A</t>
@@ -3291,34 +3291,34 @@
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr"/>
+      <c r="M15" s="3" t="inlineStr"/>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J15" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K15" s="3" t="inlineStr">
+      <c r="O15" s="3" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="L15" s="3" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M15" s="3" t="inlineStr"/>
-      <c r="N15" s="3" t="inlineStr"/>
-      <c r="O15" s="3" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
       <c r="P15" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="Q15" s="3" t="inlineStr"/>
@@ -3331,14 +3331,14 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3346,46 +3346,46 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
+      <c r="J16" s="3" t="inlineStr">
         <is>
           <t>4B</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>4A</t>
         </is>
       </c>
       <c r="K16" s="3" t="inlineStr"/>
       <c r="L16" s="3" t="inlineStr"/>
       <c r="M16" s="3" t="inlineStr"/>
-      <c r="N16" s="3" t="inlineStr"/>
-      <c r="O16" s="3" t="inlineStr">
+      <c r="N16" s="3" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
+      <c r="O16" s="3" t="inlineStr"/>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="Q16" s="3" t="inlineStr"/>
@@ -3396,7 +3396,11 @@
           <t>MER4</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr"/>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
           <t>1A</t>
@@ -3409,12 +3413,12 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
           <t>2B</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>2A</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
@@ -3445,11 +3449,7 @@
           <t>5A</t>
         </is>
       </c>
-      <c r="O17" s="3" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="O17" s="3" t="inlineStr"/>
       <c r="P17" s="3" t="inlineStr">
         <is>
           <t>4B</t>
@@ -3463,65 +3463,65 @@
           <t>MER5</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr"/>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr"/>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="H18" s="3" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I18" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J18" s="3" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K18" s="3" t="inlineStr"/>
-      <c r="L18" s="3" t="inlineStr"/>
       <c r="M18" s="3" t="inlineStr"/>
       <c r="N18" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="O18" s="3" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="P18" s="3" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="O18" s="3" t="inlineStr"/>
+      <c r="P18" s="3" t="inlineStr"/>
       <c r="Q18" s="3" t="inlineStr"/>
     </row>
     <row r="19">
@@ -3530,7 +3530,11 @@
           <t>MER6</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr"/>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
           <t>1B</t>
@@ -3543,30 +3547,34 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
           <t>3A</t>
         </is>
       </c>
-      <c r="H19" s="3" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="J19" s="3" t="inlineStr"/>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="K19" s="3" t="inlineStr"/>
       <c r="L19" s="3" t="inlineStr"/>
       <c r="M19" s="3" t="inlineStr"/>
@@ -3575,16 +3583,8 @@
           <t>5B</t>
         </is>
       </c>
-      <c r="O19" s="3" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="P19" s="3" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
+      <c r="O19" s="3" t="inlineStr"/>
+      <c r="P19" s="3" t="inlineStr"/>
       <c r="Q19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
@@ -3593,62 +3593,62 @@
           <t>GIO1</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr">
+      <c r="B20" s="4" t="inlineStr"/>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr"/>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="inlineStr"/>
+      <c r="G20" s="4" t="inlineStr"/>
+      <c r="H20" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I20" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J20" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L20" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="M20" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="N20" s="4" t="inlineStr"/>
+      <c r="O20" s="4" t="inlineStr"/>
+      <c r="P20" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="Q20" s="4" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="inlineStr"/>
-      <c r="G20" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H20" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I20" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J20" s="4" t="inlineStr"/>
-      <c r="K20" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L20" s="4" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="M20" s="4" t="inlineStr"/>
-      <c r="N20" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O20" s="4" t="inlineStr"/>
-      <c r="P20" s="4" t="inlineStr"/>
-      <c r="Q20" s="4" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
@@ -3656,65 +3656,65 @@
           <t>GIO2</t>
         </is>
       </c>
-      <c r="B21" s="4" t="inlineStr">
+      <c r="B21" s="4" t="inlineStr"/>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr"/>
+      <c r="G21" s="4" t="inlineStr"/>
+      <c r="H21" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I21" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J21" s="4" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="K21" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L21" s="4" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="M21" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="N21" s="4" t="inlineStr"/>
+      <c r="O21" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="P21" s="4" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G21" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H21" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J21" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L21" s="4" t="inlineStr"/>
-      <c r="M21" s="4" t="inlineStr"/>
-      <c r="N21" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O21" s="4" t="inlineStr"/>
-      <c r="P21" s="4" t="inlineStr"/>
       <c r="Q21" s="4" t="inlineStr"/>
     </row>
     <row r="22">
@@ -3725,14 +3725,14 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
           <t>5A</t>
@@ -3740,46 +3740,46 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr">
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="inlineStr"/>
+      <c r="G22" s="4" t="inlineStr"/>
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H22" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr"/>
       <c r="M22" s="4" t="inlineStr"/>
       <c r="N22" s="4" t="inlineStr"/>
-      <c r="O22" s="4" t="inlineStr"/>
+      <c r="O22" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="P22" s="4" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="Q22" s="4" t="inlineStr"/>
@@ -3792,14 +3792,10 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
           <t>1A</t>
         </is>
       </c>
+      <c r="C23" s="4" t="inlineStr"/>
       <c r="D23" s="4" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3812,7 +3808,7 @@
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
@@ -3843,10 +3839,14 @@
       <c r="L23" s="4" t="inlineStr"/>
       <c r="M23" s="4" t="inlineStr"/>
       <c r="N23" s="4" t="inlineStr"/>
-      <c r="O23" s="4" t="inlineStr"/>
+      <c r="O23" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="P23" s="4" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr"/>
@@ -3862,17 +3862,17 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="C24" s="4" t="inlineStr"/>
       <c r="D24" s="4" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr"/>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
           <t>2A</t>
@@ -3880,40 +3880,40 @@
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
           <t>COPERTURA</t>
         </is>
       </c>
-      <c r="H24" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I24" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
       <c r="J24" s="4" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="K24" s="4" t="inlineStr"/>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="L24" s="4" t="inlineStr"/>
-      <c r="M24" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+      <c r="M24" s="4" t="inlineStr"/>
       <c r="N24" s="4" t="inlineStr"/>
       <c r="O24" s="4" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="P24" s="4" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="Q24" s="4" t="inlineStr"/>
@@ -3929,57 +3929,57 @@
           <t>1B</t>
         </is>
       </c>
-      <c r="C25" s="4" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
+      <c r="C25" s="4" t="inlineStr"/>
       <c r="D25" s="4" t="inlineStr">
         <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H25" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I25" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J25" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K25" s="4" t="inlineStr">
+        <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="E25" s="4" t="inlineStr"/>
-      <c r="F25" s="4" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G25" s="4" t="inlineStr"/>
-      <c r="H25" s="4" t="inlineStr"/>
-      <c r="I25" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="J25" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K25" s="4" t="inlineStr"/>
       <c r="L25" s="4" t="inlineStr"/>
-      <c r="M25" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="M25" s="4" t="inlineStr"/>
       <c r="N25" s="4" t="inlineStr"/>
       <c r="O25" s="4" t="inlineStr">
         <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="P25" s="4" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="Q25" s="4" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="P25" s="4" t="inlineStr"/>
+      <c r="Q25" s="4" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
@@ -3987,7 +3987,11 @@
           <t>VEN1</t>
         </is>
       </c>
-      <c r="B26" s="5" t="inlineStr"/>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
           <t>1A</t>
@@ -3999,50 +4003,46 @@
           <t>2A</t>
         </is>
       </c>
-      <c r="F26" s="5" t="inlineStr"/>
+      <c r="F26" s="5" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
       <c r="G26" s="5" t="inlineStr"/>
-      <c r="H26" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
+      <c r="H26" s="5" t="inlineStr"/>
       <c r="I26" s="5" t="inlineStr">
         <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J26" s="5" t="inlineStr">
+        <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="J26" s="5" t="inlineStr"/>
       <c r="K26" s="5" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="L26" s="5" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
+      <c r="L26" s="5" t="inlineStr"/>
       <c r="M26" s="5" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="N26" s="5" t="inlineStr"/>
       <c r="O26" s="5" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="P26" s="5" t="inlineStr">
         <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="Q26" s="5" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="Q26" s="5" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
@@ -4050,10 +4050,14 @@
           <t>VEN2</t>
         </is>
       </c>
-      <c r="B27" s="5" t="inlineStr"/>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr"/>
@@ -4072,41 +4076,37 @@
           <t>3B</t>
         </is>
       </c>
-      <c r="H27" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
+      <c r="H27" s="5" t="inlineStr"/>
       <c r="I27" s="5" t="inlineStr">
         <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J27" s="5" t="inlineStr"/>
       <c r="K27" s="5" t="inlineStr">
         <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L27" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr"/>
       <c r="M27" s="5" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="N27" s="5" t="inlineStr"/>
       <c r="O27" s="5" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="P27" s="5" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="Q27" s="5" t="inlineStr"/>
@@ -4119,61 +4119,61 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C28" s="5" t="inlineStr"/>
       <c r="D28" s="5" t="inlineStr">
         <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H28" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I28" s="5" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J28" s="5" t="inlineStr"/>
+      <c r="K28" s="5" t="inlineStr"/>
+      <c r="L28" s="5" t="inlineStr"/>
+      <c r="M28" s="5" t="inlineStr">
+        <is>
           <t>5A</t>
-        </is>
-      </c>
-      <c r="E28" s="5" t="inlineStr"/>
-      <c r="F28" s="5" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H28" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I28" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="J28" s="5" t="inlineStr"/>
-      <c r="K28" s="5" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L28" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="M28" s="5" t="inlineStr">
-        <is>
-          <t>4B</t>
         </is>
       </c>
       <c r="N28" s="5" t="inlineStr"/>
       <c r="O28" s="5" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="P28" s="5" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="Q28" s="5" t="inlineStr"/>
@@ -4184,63 +4184,63 @@
           <t>VEN4</t>
         </is>
       </c>
-      <c r="B29" s="5" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C29" s="5" t="inlineStr"/>
+      <c r="B29" s="5" t="inlineStr"/>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr"/>
       <c r="F29" s="5" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H29" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J29" s="5" t="inlineStr"/>
+      <c r="K29" s="5" t="inlineStr"/>
+      <c r="L29" s="5" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="M29" s="5" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="N29" s="5" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="O29" s="5" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="P29" s="5" t="inlineStr">
+        <is>
           <t>2B</t>
-        </is>
-      </c>
-      <c r="G29" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H29" s="5" t="inlineStr"/>
-      <c r="I29" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J29" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K29" s="5" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L29" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="M29" s="5" t="inlineStr"/>
-      <c r="N29" s="5" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O29" s="5" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="P29" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
         </is>
       </c>
       <c r="Q29" s="5" t="inlineStr"/>
@@ -4251,47 +4251,43 @@
           <t>VEN5</t>
         </is>
       </c>
-      <c r="B30" s="5" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C30" s="5" t="inlineStr"/>
+      <c r="B30" s="5" t="inlineStr"/>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E30" s="5" t="inlineStr"/>
       <c r="F30" s="5" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="H30" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I30" s="5" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J30" s="5" t="inlineStr"/>
+      <c r="K30" s="5" t="inlineStr"/>
+      <c r="L30" s="5" t="inlineStr">
+        <is>
           <t>2B</t>
-        </is>
-      </c>
-      <c r="G30" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H30" s="5" t="inlineStr"/>
-      <c r="I30" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J30" s="5" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K30" s="5" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L30" s="5" t="inlineStr">
-        <is>
-          <t>2A</t>
         </is>
       </c>
       <c r="M30" s="5" t="inlineStr"/>
@@ -4302,15 +4298,19 @@
       </c>
       <c r="O30" s="5" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="P30" s="5" t="inlineStr">
         <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="Q30" s="5" t="inlineStr"/>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="Q30" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="inlineStr">

</xml_diff>

<commit_message>
Aggiunte modifiche CLI engine e pulizia nomi file
</commit_message>
<xml_diff>
--- a/orario_settimanale.xlsx
+++ b/orario_settimanale.xlsx
@@ -527,52 +527,52 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
+          <t>CICCIMARRA</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>RUSSO</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>ANGELINI (1h)</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>PEPE (1h)</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>CARDONE (1h)</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>PEPE (1h)</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI (1h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L2" s="1" t="inlineStr"/>
@@ -585,37 +585,37 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>CICCIMARRA (2h)</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI (2h)</t>
-        </is>
-      </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h) CARDONE (1h)</t>
+          <t>SAVINO (1h) MARANGI (1h)</t>
         </is>
       </c>
     </row>
@@ -647,57 +647,57 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE (2h)</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>CARDONE (1h)</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>LEO (2h)</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI (3h)</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
-        </is>
-      </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>ZIZZI (3h)</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>ANGELINI (1h) SABATELLI (0h 30m)</t>
+          <t>MARANGI (1h) SABATELLI (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -709,22 +709,22 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>CICCIMARRA (2h)</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>RUSSO (3h)</t>
+          <t>ANGELINI (2h)</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
@@ -734,32 +734,32 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PALMISANO (3h)</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO (2h)</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>CARDONE (2h)</t>
-        </is>
-      </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI (3h)</t>
+          <t>ZIZZI (1h)</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
     </row>
@@ -771,22 +771,22 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
           <t>RUSSO (1h 30m)</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h 30m)</t>
-        </is>
-      </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h 30m)</t>
+          <t>SCHIAVONE (2h 30m)</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>SABATELLI (1h 30m)</t>
+          <t>SABATELLI (2h 30m)</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr">
@@ -811,17 +811,17 @@
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       <c r="G7" s="1" t="inlineStr"/>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
@@ -849,12 +849,12 @@
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr"/>
@@ -867,29 +867,29 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
+          <t>ANGELINI (1h)</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
           <t>RUSSO (1h)</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI (1h)</t>
-        </is>
-      </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
           <t>SIMEONE (1h)</t>
@@ -897,17 +897,17 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -925,57 +925,57 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>RUSSO (1h)</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (1h)</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (1h)</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>PEPE (2h)</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>OSTUNI (2h)</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI (2h)</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
         <is>
           <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="I9" s="2" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J9" s="2" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>RUSSO (1h)</t>
         </is>
       </c>
     </row>
@@ -987,57 +987,57 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>ANGELINI (2h)</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>SIMEONE (2h)</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>CARDONE (1h)</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>OSTUNI (1h)</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
+        <is>
           <t>RUSSO (1h)</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI (2h)</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>MARANGI (2h)</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="I10" s="2" t="inlineStr">
-        <is>
-          <t>PEPE (2h)</t>
-        </is>
-      </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI (3h)</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h)</t>
         </is>
       </c>
     </row>
@@ -1049,57 +1049,57 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA (2h)</t>
+          <t>SCHIAVONE (2h)</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h)</t>
+          <t>SABATELLI (2h)</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE (3h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
+          <t>PALMISANO (1h)</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>PEPE (2h)</t>
+        </is>
+      </c>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
           <t>MOTORIA (1h)</t>
         </is>
       </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>PALMISANO (1h)</t>
-        </is>
-      </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>MARANGI (1h) PEPE (1h)</t>
+          <t>MARANGI (1h) ANGELINI (1h)</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (1h 30m)</t>
+          <t>RUSSO (2h 30m)</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
@@ -1121,14 +1121,14 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
+          <t>SABATELLI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
           <t>SCHIAVONE (1h 30m)</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h 30m)</t>
-        </is>
-      </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
           <t>MARANGI (1h 30m)</t>
@@ -1136,32 +1136,32 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE (1h 30m)</t>
+          <t>SIMEONE (2h 30m)</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>MOTORIA (1h)</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>ZIZZI (3h)</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="I12" s="2" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
       <c r="L12" s="2" t="inlineStr">
         <is>
-          <t>PALMISANO (1h) CARDONE (0h 30m)</t>
+          <t>CARDONE (1h) PALMISANO (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -1179,22 +1179,22 @@
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="2" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
           <t>PALMISANO (1h)</t>
         </is>
       </c>
-      <c r="I13" s="2" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="K13" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI (3h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="L13" s="2" t="inlineStr"/>
@@ -1207,27 +1207,27 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
+          <t>RUSSO (1h)</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
           <t>ANGELINI</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SIMEONE (1h)</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
@@ -1237,22 +1237,22 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>PEPE (1h)</t>
-        </is>
-      </c>
       <c r="J14" s="3" t="inlineStr">
         <is>
+          <t>ZIZZI (1h)</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
           <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>ZIZZI (1h)</t>
         </is>
       </c>
       <c r="L14" s="3" t="inlineStr"/>
@@ -1265,57 +1265,57 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>ANGELINI (2h)</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SCHIAVONE (1h)</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>PALMISANO (2h)</t>
+          <t>PEPE (2h)</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
+          <t>CARDONE</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
           <t>ZIZZI (1h)</t>
         </is>
       </c>
-      <c r="K15" s="3" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>PEPE (1h) MARANGI (1h)</t>
+          <t>SABATELLI (1h) RUSSO (1h)</t>
         </is>
       </c>
     </row>
@@ -1327,12 +1327,12 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI (3h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>RUSSO (2h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -1342,42 +1342,42 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE (2h)</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="H16" s="3" t="inlineStr">
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO (3h)</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>CARDONE</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>OSTUNI</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI (1h) SABATELLI (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -1389,57 +1389,57 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>RUSSO</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (2h)</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI (3h)</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE (3h)</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>ANGELINI (1h)</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (3h)</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (2h)</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H17" s="3" t="inlineStr">
-        <is>
-          <t>PEPE (2h)</t>
-        </is>
-      </c>
-      <c r="I17" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>CARDONE (3h)</t>
         </is>
       </c>
       <c r="K17" s="3" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L17" s="3" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1451,12 +1451,12 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>RUSSO (1h 30m)</t>
+          <t>ANGELINI (3h 30m)</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h 30m)</t>
+          <t>RUSSO (3h 30m)</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
@@ -1471,37 +1471,37 @@
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>MARANGI (2h 30m)</t>
+          <t>SIMEONE (1h 30m)</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE (2h 30m)</t>
+          <t>MARANGI (1h 30m)</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
           <t>CARDONE (1h)</t>
         </is>
       </c>
-      <c r="I18" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="L18" s="3" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>PEPE (3h)</t>
         </is>
       </c>
     </row>
@@ -1519,22 +1519,22 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PALMISANO (3h)</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>PALMISANO (3h)</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>LEO (2h)</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="L19" s="3" t="inlineStr"/>
@@ -1547,12 +1547,12 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
       <c r="D20" s="4" t="inlineStr">
@@ -1567,17 +1567,17 @@
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SIMEONE (1h)</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -1605,37 +1605,37 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>CICCIMARRA (2h)</t>
         </is>
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (2h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G21" s="4" t="inlineStr">
-        <is>
-          <t>MARANGI (2h)</t>
-        </is>
-      </c>
       <c r="H21" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="I21" s="4" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L21" s="4" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
     </row>
@@ -1667,42 +1667,42 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI (3h)</t>
+          <t>RUSSO (1h)</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>RUSSO (3h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h)</t>
+          <t>SABATELLI (3h)</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO (3h)</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="L22" s="4" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
     </row>
@@ -1729,42 +1729,42 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>RUSSO (1h)</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (3h)</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE (3h)</t>
-        </is>
-      </c>
-      <c r="G23" s="4" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="H23" s="4" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PALMISANO (2h)</t>
         </is>
       </c>
       <c r="J23" s="4" t="inlineStr">
@@ -1791,42 +1791,42 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>RUSSO (2h 30m)</t>
+          <t>RUSSO (1h 30m)</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI (2h 30m)</t>
+          <t>ANGELINI (1h 30m)</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
+          <t>SCHIAVONE (1h 30m)</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
           <t>SABATELLI (1h 30m)</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (2h 30m)</t>
-        </is>
-      </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>MARANGI (1h 30m)</t>
+          <t>SIMEONE (2h 30m)</t>
         </is>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE (1h 30m)</t>
+          <t>MARANGI (2h 30m)</t>
         </is>
       </c>
       <c r="H24" s="4" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="I24" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="J24" s="4" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="K24" s="4" t="inlineStr">
         <is>
-          <t>ZIZZI (2h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L24" s="4" t="inlineStr">
         <is>
-          <t>SAVINO (1h) CARDONE (0h 30m)</t>
+          <t>PEPE (1h) PALMISANO (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -1859,12 +1859,12 @@
       <c r="G25" s="4" t="inlineStr"/>
       <c r="H25" s="4" t="inlineStr">
         <is>
-          <t>PEPE (2h)</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO (3h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="J25" s="4" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="K25" s="4" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>ZIZZI (3h)</t>
         </is>
       </c>
       <c r="L25" s="4" t="inlineStr"/>
@@ -1887,42 +1887,42 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
+          <t>RUSSO (1h)</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>ANGELINI (1h)</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="F26" s="5" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="C26" s="5" t="inlineStr">
-        <is>
-          <t>RUSSO (1h)</t>
-        </is>
-      </c>
-      <c r="D26" s="5" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="E26" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="F26" s="5" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>SIMEONE (1h)</t>
         </is>
       </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I26" s="5" t="inlineStr">
+        <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I26" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO (1h)</t>
         </is>
       </c>
       <c r="J26" s="5" t="inlineStr">
@@ -1945,44 +1945,44 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
           <t>RUSSO (1h)</t>
         </is>
       </c>
-      <c r="C27" s="5" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>SABATELLI (1h)</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SCHIAVONE (1h)</t>
         </is>
       </c>
       <c r="F27" s="5" t="inlineStr">
         <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="G27" s="5" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H27" s="5" t="inlineStr">
         <is>
+          <t>PALMISANO (2h)</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
           <t>PEPE (2h)</t>
         </is>
       </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
       <c r="J27" s="5" t="inlineStr">
         <is>
           <t>OSTUNI (2h)</t>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="L27" s="5" t="inlineStr">
         <is>
-          <t>PALMISANO (1h)</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
     </row>
@@ -2007,42 +2007,42 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (2h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="F28" s="5" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="G28" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE (3h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I28" s="5" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="J28" s="5" t="inlineStr">
@@ -2052,12 +2052,12 @@
       </c>
       <c r="K28" s="5" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="L28" s="5" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
     </row>
@@ -2079,34 +2079,34 @@
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>LEO (2h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h)</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="F29" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
+          <t>PEPE (2h)</t>
+        </is>
+      </c>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I29" s="5" t="inlineStr">
-        <is>
-          <t>PEPE (2h)</t>
-        </is>
-      </c>
       <c r="J29" s="5" t="inlineStr">
         <is>
           <t>ZIZZI</t>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="L29" s="5" t="inlineStr">
@@ -2131,44 +2131,44 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (2h)</t>
+          <t>ANGELINI (3h)</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (3h)</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="D30" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (1h)</t>
-        </is>
-      </c>
-      <c r="E30" s="5" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
       <c r="F30" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE (2h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="H30" s="5" t="inlineStr">
         <is>
+          <t>MOTORIA (1h)</t>
+        </is>
+      </c>
+      <c r="I30" s="5" t="inlineStr">
+        <is>
           <t>PALMISANO (2h)</t>
         </is>
       </c>
-      <c r="I30" s="5" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
       <c r="J30" s="5" t="inlineStr">
         <is>
           <t>ZIZZI (3h)</t>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="L30" s="5" t="inlineStr">
@@ -2386,26 +2386,26 @@
           <t>LUN1</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr"/>
+      <c r="B2" s="1" t="inlineStr"/>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr"/>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr"/>
@@ -2417,28 +2417,28 @@
       <c r="J2" s="1" t="inlineStr"/>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr"/>
-      <c r="M2" s="1" t="inlineStr">
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr"/>
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>4B (1h)</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -2448,14 +2448,10 @@
           <t>LUN2</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
+      <c r="B3" s="1" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1B (2h)</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -2465,17 +2461,17 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>2B (2h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr"/>
@@ -2484,26 +2480,30 @@
           <t>4B (1h)</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr"/>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="L3" s="1" t="inlineStr"/>
-      <c r="M3" s="1" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>1A (2h)</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr"/>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="P3" s="1" t="inlineStr">
@@ -2520,17 +2520,17 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5A (3h)</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -2540,12 +2540,12 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>2A (2h)</t>
+          <t>2B (2h)</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>3B (3h)</t>
+          <t>COPERTURA (2h)</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr"/>
@@ -2557,32 +2557,28 @@
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5B (3h)</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="M4" s="1" t="inlineStr">
-        <is>
-          <t>BUCO</t>
-        </is>
-      </c>
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="M4" s="1" t="inlineStr"/>
       <c r="N4" s="1" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="O4" s="1" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="P4" s="1" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -2594,32 +2590,32 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>BUCO (1h)</t>
+          <t>1B (2h)</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>1B (3h)</t>
+          <t>1A (2h)</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>5A (3h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -2630,39 +2626,27 @@
       <c r="I5" s="1" t="inlineStr"/>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>4A (3h)</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
-        <is>
-          <t>1A (2h)</t>
-        </is>
-      </c>
-      <c r="M5" s="1" t="inlineStr">
-        <is>
-          <t>BUCO (2h)</t>
-        </is>
-      </c>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr"/>
+      <c r="M5" s="1" t="inlineStr"/>
       <c r="N5" s="1" t="inlineStr">
         <is>
-          <t>4B (2h)</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="O5" s="1" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="P5" s="1" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="P5" s="1" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2672,23 +2656,27 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>1A (1h 30m)</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>1A (1h 30m)</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr"/>
+          <t>1B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>2B (1h 30m)</t>
+          <t>2B (2h 30m)</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>2A (1h 30m)</t>
+          <t>2A (2h 30m)</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
@@ -2708,31 +2696,23 @@
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr"/>
-      <c r="L6" s="1" t="inlineStr">
-        <is>
-          <t>1B (1h 30m)</t>
-        </is>
-      </c>
+      <c r="L6" s="1" t="inlineStr"/>
       <c r="M6" s="1" t="inlineStr">
         <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="N6" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA (2h)</t>
+        </is>
+      </c>
+      <c r="O6" s="1" t="inlineStr">
+        <is>
           <t>5A (1h)</t>
         </is>
       </c>
-      <c r="N6" s="1" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
-      <c r="O6" s="1" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="P6" s="1" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
+      <c r="P6" s="1" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2742,7 +2722,11 @@
       </c>
       <c r="B7" s="1" t="inlineStr"/>
       <c r="C7" s="1" t="inlineStr"/>
-      <c r="D7" s="1" t="inlineStr"/>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>5B (3h)</t>
+        </is>
+      </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr"/>
       <c r="G7" s="1" t="inlineStr"/>
@@ -2757,19 +2741,15 @@
       <c r="L7" s="1" t="inlineStr"/>
       <c r="M7" s="1" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5A (1h)</t>
         </is>
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="O7" s="1" t="inlineStr">
-        <is>
           <t>4A (1h)</t>
         </is>
       </c>
+      <c r="O7" s="1" t="inlineStr"/>
       <c r="P7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
@@ -2778,15 +2758,19 @@
           <t>MAR1</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
@@ -2795,11 +2779,7 @@
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr"/>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
+      <c r="G8" s="2" t="inlineStr"/>
       <c r="H8" s="2" t="inlineStr">
         <is>
           <t>3B (1h)</t>
@@ -2807,7 +2787,7 @@
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr"/>
@@ -2816,21 +2796,21 @@
           <t>5B</t>
         </is>
       </c>
-      <c r="L8" s="2" t="inlineStr"/>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>2B (1h)</t>
+        </is>
+      </c>
       <c r="M8" s="2" t="inlineStr"/>
       <c r="N8" s="2" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="O8" s="2" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="O8" s="2" t="inlineStr"/>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
     </row>
@@ -2847,29 +2827,25 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>5A (2h)</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>BUCO</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
+      <c r="G9" s="2" t="inlineStr"/>
       <c r="H9" s="2" t="inlineStr">
         <is>
           <t>3A</t>
@@ -2877,34 +2853,30 @@
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A (2h)</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr"/>
       <c r="K9" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L9" s="2" t="inlineStr"/>
-      <c r="M9" s="2" t="inlineStr">
-        <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
+          <t>5B (2h)</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="M9" s="2" t="inlineStr"/>
       <c r="N9" s="2" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="O9" s="2" t="inlineStr">
-        <is>
-          <t>BUCO</t>
-        </is>
-      </c>
+          <t>4B (2h)</t>
+        </is>
+      </c>
+      <c r="O9" s="2" t="inlineStr"/>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -2921,68 +2893,56 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>BUCO (2h)</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>3B (2h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3A (2h)</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>4B (2h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr"/>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr"/>
+      <c r="M10" s="2" t="inlineStr"/>
       <c r="N10" s="2" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="O10" s="2" t="inlineStr">
-        <is>
-          <t>BUCO</t>
-        </is>
-      </c>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="O10" s="2" t="inlineStr"/>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
     </row>
@@ -2994,77 +2954,65 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr"/>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>2B (2h)</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>2A (2h)</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>4B (2h)</t>
+        </is>
+      </c>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L11" s="2" t="inlineStr"/>
+      <c r="M11" s="2" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="N11" s="2" t="inlineStr">
+        <is>
+          <t>3A (1h)</t>
+        </is>
+      </c>
+      <c r="O11" s="2" t="inlineStr"/>
+      <c r="P11" s="2" t="inlineStr">
+        <is>
           <t>1B (1h)</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>2B (2h)</t>
-        </is>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>3A (3h)</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L11" s="2" t="inlineStr">
-        <is>
-          <t>2A (2h)</t>
-        </is>
-      </c>
-      <c r="M11" s="2" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="N11" s="2" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
-      <c r="O11" s="2" t="inlineStr">
-        <is>
-          <t>BUCO (3h)</t>
-        </is>
-      </c>
-      <c r="P11" s="2" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -3081,24 +3029,20 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>1A (1h 30m)</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+          <t>1A (2h 30m)</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr"/>
       <c r="E12" s="2" t="inlineStr">
         <is>
+          <t>2A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
           <t>2B (1h 30m)</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>2A (1h 30m)</t>
-        </is>
-      </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
           <t>3A (1h 30m)</t>
@@ -3106,35 +3050,39 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>3B (1h 30m)</t>
+          <t>3B (2h 30m)</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr">
         <is>
+          <t>COPERTURA (0h 30m)</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>5A (3h)</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr"/>
+      <c r="M12" s="2" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="N12" s="2" t="inlineStr">
+        <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L12" s="2" t="inlineStr"/>
-      <c r="M12" s="2" t="inlineStr"/>
-      <c r="N12" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (0h 30m)</t>
-        </is>
-      </c>
       <c r="O12" s="2" t="inlineStr">
         <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="P12" s="2" t="inlineStr">
+        <is>
           <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="P12" s="2" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -3146,11 +3094,7 @@
       </c>
       <c r="B13" s="2" t="inlineStr"/>
       <c r="C13" s="2" t="inlineStr"/>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>5B (3h)</t>
-        </is>
-      </c>
+      <c r="D13" s="2" t="inlineStr"/>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="2" t="inlineStr"/>
       <c r="G13" s="2" t="inlineStr"/>
@@ -3158,20 +3102,24 @@
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr">
         <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr"/>
+      <c r="L13" s="2" t="inlineStr"/>
+      <c r="M13" s="2" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="N13" s="2" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
           <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>5A (3h)</t>
-        </is>
-      </c>
-      <c r="L13" s="2" t="inlineStr"/>
-      <c r="M13" s="2" t="inlineStr"/>
-      <c r="N13" s="2" t="inlineStr"/>
-      <c r="O13" s="2" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
         </is>
       </c>
       <c r="P13" s="2" t="inlineStr"/>
@@ -3184,57 +3132,57 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr"/>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
       <c r="D14" s="3" t="inlineStr"/>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E14" s="3" t="inlineStr"/>
+      <c r="F14" s="3" t="inlineStr"/>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>3B (1h)</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>3A (1h)</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
         <is>
           <t>2A (1h)</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="H14" s="3" t="inlineStr"/>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="J14" s="3" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="L14" s="3" t="inlineStr"/>
       <c r="M14" s="3" t="inlineStr"/>
       <c r="N14" s="3" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="O14" s="3" t="inlineStr">
-        <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr"/>
       <c r="P14" s="3" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
     </row>
@@ -3246,65 +3194,65 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B (2h)</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="3" t="inlineStr">
         <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>4A (2h)</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K15" s="3" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="L15" s="3" t="inlineStr"/>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
       <c r="M15" s="3" t="inlineStr"/>
       <c r="N15" s="3" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="O15" s="3" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="O15" s="3" t="inlineStr"/>
       <c r="P15" s="3" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
     </row>
@@ -3316,22 +3264,22 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>1A (3h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>1B (2h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (0h 30m)</t>
+          <t>COPERTURA (1h 30m)</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
@@ -3341,44 +3289,40 @@
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
         <is>
-          <t>BUCO (1h)</t>
+          <t>4B (3h)</t>
         </is>
       </c>
       <c r="K16" s="3" t="inlineStr"/>
       <c r="L16" s="3" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="M16" s="3" t="inlineStr"/>
       <c r="N16" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="O16" s="3" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="O16" s="3" t="inlineStr"/>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
     </row>
@@ -3390,69 +3334,61 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>BUCO (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>2A (3h)</t>
+          <t>2A (2h)</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3A (3h)</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3B (3h)</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="K17" s="3" t="inlineStr"/>
-      <c r="L17" s="3" t="inlineStr">
-        <is>
-          <t>2B (2h)</t>
-        </is>
-      </c>
+      <c r="L17" s="3" t="inlineStr"/>
       <c r="M17" s="3" t="inlineStr"/>
       <c r="N17" s="3" t="inlineStr">
         <is>
-          <t>5B (2h)</t>
-        </is>
-      </c>
-      <c r="O17" s="3" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
+          <t>5A (3h)</t>
+        </is>
+      </c>
+      <c r="O17" s="3" t="inlineStr"/>
       <c r="P17" s="3" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -3462,15 +3398,19 @@
           <t>MER5</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr"/>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>1A (3h 30m)</t>
+        </is>
+      </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>1A (1h 30m)</t>
+          <t>1B (3h 30m)</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5B (3h)</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
@@ -3485,46 +3425,38 @@
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>3A (2h 30m)</t>
+          <t>3B (1h 30m)</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>3B (2h 30m)</t>
+          <t>3A (1h 30m)</t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>COPERTURA (3h)</t>
         </is>
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr"/>
-      <c r="L18" s="3" t="inlineStr">
-        <is>
-          <t>1B (1h 30m)</t>
-        </is>
-      </c>
+      <c r="L18" s="3" t="inlineStr"/>
       <c r="M18" s="3" t="inlineStr"/>
       <c r="N18" s="3" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="O18" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="P18" s="3" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="P18" s="3" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -3536,17 +3468,21 @@
       <c r="C19" s="3" t="inlineStr"/>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>5B (2h)</t>
+          <t>5A (1h)</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
       <c r="F19" s="3" t="inlineStr"/>
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr"/>
-      <c r="I19" s="3" t="inlineStr"/>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>4B (3h)</t>
+          <t>4A (3h)</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr"/>
@@ -3555,14 +3491,10 @@
       <c r="N19" s="3" t="inlineStr"/>
       <c r="O19" s="3" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
-        </is>
-      </c>
-      <c r="P19" s="3" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="P19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
@@ -3570,16 +3502,8 @@
           <t>GIO1</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="B20" s="4" t="inlineStr"/>
+      <c r="C20" s="4" t="inlineStr"/>
       <c r="D20" s="4" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3593,28 +3517,36 @@
       <c r="F20" s="4" t="inlineStr"/>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="H20" s="4" t="inlineStr"/>
+          <t>3B (1h)</t>
+        </is>
+      </c>
+      <c r="H20" s="4" t="inlineStr">
+        <is>
+          <t>3A (1h)</t>
+        </is>
+      </c>
       <c r="I20" s="4" t="inlineStr">
         <is>
           <t>4B</t>
         </is>
       </c>
-      <c r="J20" s="4" t="inlineStr">
+      <c r="J20" s="4" t="inlineStr"/>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L20" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="M20" s="4" t="inlineStr"/>
+      <c r="N20" s="4" t="inlineStr">
         <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="K20" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L20" s="4" t="inlineStr"/>
-      <c r="M20" s="4" t="inlineStr"/>
-      <c r="N20" s="4" t="inlineStr"/>
       <c r="O20" s="4" t="inlineStr">
         <is>
           <t>2B (1h)</t>
@@ -3622,7 +3554,7 @@
       </c>
       <c r="P20" s="4" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
     </row>
@@ -3632,16 +3564,8 @@
           <t>GIO2</t>
         </is>
       </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="B21" s="4" t="inlineStr"/>
+      <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="4" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3649,22 +3573,22 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>2A (2h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>3B (2h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="H21" s="4" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I21" s="4" t="inlineStr">
@@ -3672,31 +3596,31 @@
           <t>4B (2h)</t>
         </is>
       </c>
-      <c r="J21" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
+      <c r="J21" s="4" t="inlineStr"/>
       <c r="K21" s="4" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="L21" s="4" t="inlineStr"/>
+      <c r="L21" s="4" t="inlineStr">
+        <is>
+          <t>1B (2h)</t>
+        </is>
+      </c>
       <c r="M21" s="4" t="inlineStr"/>
       <c r="N21" s="4" t="inlineStr">
         <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
+      <c r="O21" s="4" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="P21" s="4" t="inlineStr">
+        <is>
           <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="O21" s="4" t="inlineStr">
-        <is>
-          <t>BUCO</t>
-        </is>
-      </c>
-      <c r="P21" s="4" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
         </is>
       </c>
     </row>
@@ -3706,14 +3630,10 @@
           <t>GIO3</t>
         </is>
       </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>1A (3h)</t>
-        </is>
-      </c>
+      <c r="B22" s="4" t="inlineStr"/>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>1B (3h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
@@ -3723,32 +3643,32 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2A (3h)</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>BUCO</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B (2h)</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>4A (1h)</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>4A (3h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
@@ -3758,19 +3678,15 @@
       </c>
       <c r="L22" s="4" t="inlineStr"/>
       <c r="M22" s="4" t="inlineStr"/>
-      <c r="N22" s="4" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
+      <c r="N22" s="4" t="inlineStr"/>
       <c r="O22" s="4" t="inlineStr">
         <is>
-          <t>BUCO (2h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="P22" s="4" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
     </row>
@@ -3782,12 +3698,12 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
@@ -3802,27 +3718,27 @@
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2B (3h)</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>BUCO (2h)</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
-          <t>3A (3h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="J23" s="4" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4B (2h)</t>
         </is>
       </c>
       <c r="K23" s="4" t="inlineStr">
@@ -3832,19 +3748,15 @@
       </c>
       <c r="L23" s="4" t="inlineStr"/>
       <c r="M23" s="4" t="inlineStr"/>
-      <c r="N23" s="4" t="inlineStr">
+      <c r="N23" s="4" t="inlineStr"/>
+      <c r="O23" s="4" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="P23" s="4" t="inlineStr">
         <is>
           <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="O23" s="4" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="P23" s="4" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
         </is>
       </c>
     </row>
@@ -3856,12 +3768,12 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>1B (2h 30m)</t>
+          <t>1B (1h 30m)</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>1A (2h 30m)</t>
+          <t>1A (1h 30m)</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
@@ -3871,50 +3783,50 @@
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
+          <t>2B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
           <t>2A (1h 30m)</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
-        <is>
-          <t>2B (2h 30m)</t>
-        </is>
-      </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>3A (1h 30m)</t>
+          <t>3B (2h 30m)</t>
         </is>
       </c>
       <c r="H24" s="4" t="inlineStr">
         <is>
-          <t>3B (1h 30m)</t>
+          <t>3A (2h 30m)</t>
         </is>
       </c>
       <c r="I24" s="4" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>COPERTURA (2h)</t>
         </is>
       </c>
       <c r="J24" s="4" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>COPERTURA (0h 30m)</t>
         </is>
       </c>
       <c r="K24" s="4" t="inlineStr">
         <is>
-          <t>5B (2h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="L24" s="4" t="inlineStr"/>
       <c r="M24" s="4" t="inlineStr"/>
-      <c r="N24" s="4" t="inlineStr">
-        <is>
-          <t>COPERTURA (0h 30m)</t>
-        </is>
-      </c>
-      <c r="O24" s="4" t="inlineStr"/>
+      <c r="N24" s="4" t="inlineStr"/>
+      <c r="O24" s="4" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
       <c r="P24" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -3935,25 +3847,25 @@
       <c r="F25" s="4" t="inlineStr"/>
       <c r="G25" s="4" t="inlineStr"/>
       <c r="H25" s="4" t="inlineStr"/>
-      <c r="I25" s="4" t="inlineStr">
-        <is>
-          <t>4A (2h)</t>
-        </is>
-      </c>
+      <c r="I25" s="4" t="inlineStr"/>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>4B (3h)</t>
-        </is>
-      </c>
-      <c r="K25" s="4" t="inlineStr"/>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="K25" s="4" t="inlineStr">
+        <is>
+          <t>5B (3h)</t>
+        </is>
+      </c>
       <c r="L25" s="4" t="inlineStr"/>
       <c r="M25" s="4" t="inlineStr"/>
-      <c r="N25" s="4" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="O25" s="4" t="inlineStr"/>
+      <c r="N25" s="4" t="inlineStr"/>
+      <c r="O25" s="4" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
       <c r="P25" s="4" t="inlineStr"/>
     </row>
     <row r="26">
@@ -3962,10 +3874,14 @@
           <t>VEN1</t>
         </is>
       </c>
-      <c r="B26" s="5" t="inlineStr"/>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
@@ -3975,24 +3891,24 @@
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="F26" s="5" t="inlineStr"/>
       <c r="G26" s="5" t="inlineStr"/>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J26" s="5" t="inlineStr">
+        <is>
           <t>4A</t>
-        </is>
-      </c>
-      <c r="J26" s="5" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
         </is>
       </c>
       <c r="K26" s="5" t="inlineStr">
@@ -4002,19 +3918,15 @@
       </c>
       <c r="L26" s="5" t="inlineStr"/>
       <c r="M26" s="5" t="inlineStr"/>
-      <c r="N26" s="5" t="inlineStr">
+      <c r="N26" s="5" t="inlineStr"/>
+      <c r="O26" s="5" t="inlineStr">
         <is>
           <t>3A (1h)</t>
         </is>
       </c>
-      <c r="O26" s="5" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
       <c r="P26" s="5" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
     </row>
@@ -4026,12 +3938,12 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
@@ -4041,50 +3953,46 @@
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="F27" s="5" t="inlineStr"/>
       <c r="G27" s="5" t="inlineStr"/>
       <c r="H27" s="5" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I27" s="5" t="inlineStr">
         <is>
+          <t>4B (2h)</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
           <t>4A (2h)</t>
         </is>
       </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
       <c r="K27" s="5" t="inlineStr">
         <is>
           <t>5B (2h)</t>
         </is>
       </c>
-      <c r="L27" s="5" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
+      <c r="L27" s="5" t="inlineStr"/>
       <c r="M27" s="5" t="inlineStr"/>
-      <c r="N27" s="5" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
+      <c r="N27" s="5" t="inlineStr"/>
       <c r="O27" s="5" t="inlineStr">
         <is>
-          <t>BUCO (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="P27" s="5" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -4096,73 +4004,61 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>1B (2h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr"/>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
-      <c r="E28" s="5" t="inlineStr">
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr"/>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr"/>
+      <c r="H28" s="5" t="inlineStr">
+        <is>
+          <t>3A (2h)</t>
+        </is>
+      </c>
+      <c r="I28" s="5" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J28" s="5" t="inlineStr">
         <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="F28" s="5" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
-      <c r="H28" s="5" t="inlineStr">
-        <is>
-          <t>3B (3h)</t>
-        </is>
-      </c>
-      <c r="I28" s="5" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J28" s="5" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
       <c r="K28" s="5" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="L28" s="5" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
+      <c r="L28" s="5" t="inlineStr"/>
       <c r="M28" s="5" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="N28" s="5" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="O28" s="5" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="P28" s="5" t="inlineStr">
         <is>
-          <t>BUCO (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
     </row>
@@ -4178,60 +4074,52 @@
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr"/>
-      <c r="D29" s="5" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="D29" s="5" t="inlineStr"/>
       <c r="E29" s="5" t="inlineStr"/>
       <c r="F29" s="5" t="inlineStr">
         <is>
-          <t>2B (2h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
+          <t>3A (1h)</t>
+        </is>
+      </c>
+      <c r="H29" s="5" t="inlineStr"/>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
+      <c r="J29" s="5" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K29" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L29" s="5" t="inlineStr">
+        <is>
+          <t>2B (1h)</t>
+        </is>
+      </c>
+      <c r="M29" s="5" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="N29" s="5" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="O29" s="5" t="inlineStr">
+        <is>
           <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="H29" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I29" s="5" t="inlineStr">
-        <is>
-          <t>4B (2h)</t>
-        </is>
-      </c>
-      <c r="J29" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K29" s="5" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L29" s="5" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
-      <c r="M29" s="5" t="inlineStr">
-        <is>
-          <t>BUCO (1h)</t>
-        </is>
-      </c>
-      <c r="N29" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="O29" s="5" t="inlineStr">
-        <is>
-          <t>2A (2h)</t>
         </is>
       </c>
       <c r="P29" s="5" t="inlineStr">
@@ -4248,27 +4136,23 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>1A (2h)</t>
+          <t>1A (3h)</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr"/>
-      <c r="D30" s="5" t="inlineStr">
-        <is>
-          <t>5B (2h)</t>
-        </is>
-      </c>
+      <c r="D30" s="5" t="inlineStr"/>
       <c r="E30" s="5" t="inlineStr"/>
       <c r="F30" s="5" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
-      <c r="G30" s="5" t="inlineStr"/>
-      <c r="H30" s="5" t="inlineStr">
-        <is>
-          <t>3A (2h)</t>
-        </is>
-      </c>
+          <t>2A (3h)</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>3B (1h)</t>
+        </is>
+      </c>
+      <c r="H30" s="5" t="inlineStr"/>
       <c r="I30" s="5" t="inlineStr">
         <is>
           <t>COPERTURA (1h)</t>
@@ -4276,7 +4160,7 @@
       </c>
       <c r="J30" s="5" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>4B (2h)</t>
         </is>
       </c>
       <c r="K30" s="5" t="inlineStr">
@@ -4286,23 +4170,27 @@
       </c>
       <c r="L30" s="5" t="inlineStr">
         <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="M30" s="5" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="N30" s="5" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="O30" s="5" t="inlineStr">
+        <is>
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="M30" s="5" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="N30" s="5" t="inlineStr"/>
-      <c r="O30" s="5" t="inlineStr">
-        <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
       <c r="P30" s="5" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ore per docente per classe
</commit_message>
<xml_diff>
--- a/orario_settimanale.xlsx
+++ b/orario_settimanale.xlsx
@@ -527,52 +527,52 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>RUSSO (1h)</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>MARANGI (1h)</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
+          <t>PALMISANO (1h)</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
           <t>PEPE (1h)</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>CARDONE (1h)</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="L2" s="1" t="inlineStr"/>
@@ -585,42 +585,42 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>CICCIMARRA (2h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>RUSSO (2h)</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SABATELLI (2h)</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h) MARANGI (1h)</t>
+          <t>CARDONE (1h) RUSSO (1h)</t>
         </is>
       </c>
     </row>
@@ -647,27 +647,27 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
           <t>RUSSO</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>SCHIAVONE (2h)</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -677,27 +677,27 @@
       </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI (3h)</t>
+          <t>OSTUNI (2h)</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>MARANGI (1h) SABATELLI (0h 30m)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
     </row>
@@ -709,57 +709,57 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI (1h)</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
           <t>RUSSO (2h)</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>ANGELINI (2h)</t>
-        </is>
-      </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
+          <t>MARANGI (3h)</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
           <t>SIMEONE (1h)</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI (1h)</t>
-        </is>
-      </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>PALMISANO (3h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI (1h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>ZIZZI (3h)</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
         <is>
-          <t>CARDONE</t>
+          <t>SABATELLI (2h)</t>
         </is>
       </c>
     </row>
@@ -771,57 +771,57 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
+          <t>RUSSO (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
           <t>ANGELINI (1h 30m)</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>RUSSO (1h 30m)</t>
-        </is>
-      </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
+          <t>SABATELLI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
           <t>SCHIAVONE (2h 30m)</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI (2h 30m)</t>
-        </is>
-      </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
+          <t>SIMEONE (1h 30m)</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
           <t>MARANGI (1h 30m)</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE (1h 30m)</t>
-        </is>
-      </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
           <t>MOTORIA (1h)</t>
         </is>
       </c>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
       <c r="L6" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
     </row>
@@ -839,22 +839,22 @@
       <c r="G7" s="1" t="inlineStr"/>
       <c r="H7" s="1" t="inlineStr">
         <is>
+          <t>LEO (2h)</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>MOTORIA (1h)</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>ZIZZI (2h)</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
           <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO (2h)</t>
-        </is>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr"/>
@@ -867,32 +867,32 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>CICCIMARRA</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE (1h)</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
@@ -925,32 +925,32 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>CICCIMARRA (2h)</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -965,17 +965,17 @@
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="K9" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI (2h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>MARANGI</t>
         </is>
       </c>
     </row>
@@ -987,57 +987,57 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>ANGELINI (3h)</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>RUSSO (3h)</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>ANGELINI (2h)</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE (2h)</t>
-        </is>
-      </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI (1h)</t>
+          <t>ZIZZI (3h)</t>
         </is>
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>MARANGI (2h)</t>
         </is>
       </c>
     </row>
@@ -1054,39 +1054,39 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>SABATELLI (2h)</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (3h)</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>SIMEONE (2h)</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (2h)</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI (2h)</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>PALMISANO (1h)</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>PEPE (2h)</t>
-        </is>
-      </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
           <t>ZIZZI</t>
@@ -1094,12 +1094,12 @@
       </c>
       <c r="K11" s="2" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>MARANGI (1h) ANGELINI (1h)</t>
+          <t>PALMISANO (1h) PEPE (1h)</t>
         </is>
       </c>
     </row>
@@ -1116,32 +1116,32 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI (1h 30m)</t>
+          <t>ANGELINI (2h 30m)</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
+          <t>SCHIAVONE (1h 30m)</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
           <t>SABATELLI (1h 30m)</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (1h 30m)</t>
-        </is>
-      </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
+          <t>SIMEONE (1h 30m)</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
           <t>MARANGI (1h 30m)</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>SIMEONE (2h 30m)</t>
-        </is>
-      </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
@@ -1151,17 +1151,17 @@
       </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L12" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (1h) PALMISANO (0h 30m)</t>
+          <t>CARDONE (1h) SAVINO (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr">
@@ -1189,12 +1189,12 @@
       </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>ZIZZI (3h)</t>
         </is>
       </c>
       <c r="K13" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="L13" s="2" t="inlineStr"/>
@@ -1207,52 +1207,52 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
           <t>RUSSO (1h)</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>ANGELINI</t>
-        </is>
-      </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
           <t>CICCIMARRA (1h)</t>
         </is>
       </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="F14" s="3" t="inlineStr">
         <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE (1h)</t>
-        </is>
-      </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>MARANGI</t>
         </is>
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
           <t>PEPE</t>
         </is>
       </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
       <c r="J14" s="3" t="inlineStr">
         <is>
+          <t>CARDONE (1h)</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
           <t>ZIZZI (1h)</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="L14" s="3" t="inlineStr"/>
@@ -1265,17 +1265,17 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
           <t>CICCIMARRA (1h)</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>ANGELINI (2h)</t>
-        </is>
-      </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
@@ -1285,32 +1285,32 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI (2h)</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>PEPE (2h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
-          <t>CARDONE</t>
+          <t>ZIZZI (1h)</t>
         </is>
       </c>
       <c r="K15" s="3" t="inlineStr">
         <is>
-          <t>ZIZZI (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L15" s="3" t="inlineStr">
@@ -1327,12 +1327,12 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -1342,42 +1342,42 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE (1h)</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO (3h)</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>PEPE (3h)</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>OSTUNI</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
           <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO (3h)</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1389,57 +1389,57 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>MARANGI (3h)</t>
+          <t>SIMEONE (1h)</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE (3h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I17" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
-          <t>CARDONE (3h)</t>
+          <t>LEO (2h)</t>
         </is>
       </c>
       <c r="K17" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="L17" s="3" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>MARANGI (2h)</t>
         </is>
       </c>
     </row>
@@ -1451,57 +1451,57 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI (3h 30m)</t>
+          <t>ANGELINI (1h 30m)</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>RUSSO (3h 30m)</t>
+          <t>RUSSO (1h 30m)</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI (1h 30m)</t>
+          <t>SCHIAVONE (3h 30m)</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h 30m)</t>
+          <t>SABATELLI (3h 30m)</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
+          <t>MARANGI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
           <t>SIMEONE (1h 30m)</t>
         </is>
       </c>
-      <c r="G18" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI (1h 30m)</t>
-        </is>
-      </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
           <t>PALMISANO</t>
         </is>
       </c>
-      <c r="I18" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI (3h)</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="L18" s="3" t="inlineStr">
         <is>
-          <t>PEPE (3h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
     </row>
@@ -1519,22 +1519,22 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
+          <t>PEPE (3h)</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
           <t>PALMISANO (3h)</t>
         </is>
       </c>
-      <c r="I19" s="3" t="inlineStr">
-        <is>
-          <t>PEPE (1h)</t>
-        </is>
-      </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI (1h)</t>
+          <t>OSTUNI (2h)</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>LEO (2h)</t>
         </is>
       </c>
       <c r="L19" s="3" t="inlineStr"/>
@@ -1547,37 +1547,37 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
+          <t>ANGELINI (1h)</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>CICCIMARRA</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE (1h)</t>
-        </is>
-      </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>CARDONE</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -1605,37 +1605,37 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
+          <t>CICCIMARRA</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (1h)</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (2h)</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>MARANGI (1h)</t>
-        </is>
-      </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="H21" s="4" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>PALMISANO (2h)</t>
         </is>
       </c>
       <c r="I21" s="4" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L21" s="4" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SABATELLI (1h)</t>
         </is>
       </c>
     </row>
@@ -1667,44 +1667,44 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>CICCIMARRA (2h)</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (1h)</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>PEPE (1h)</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="D22" s="4" t="inlineStr">
-        <is>
-          <t>SABATELLI (3h)</t>
-        </is>
-      </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="G22" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE (2h)</t>
-        </is>
-      </c>
-      <c r="H22" s="4" t="inlineStr">
-        <is>
-          <t>PEPE (1h)</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
           <t>ZIZZI (3h)</t>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="L22" s="4" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
     </row>
@@ -1729,32 +1729,32 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>RUSSO (1h)</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>ANGELINI (3h)</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE (3h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="H23" s="4" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO (2h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J23" s="4" t="inlineStr">
@@ -1779,7 +1779,7 @@
       </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (1h) PEPE (1h)</t>
+          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -1791,42 +1791,42 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
+          <t>ANGELINI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
           <t>RUSSO (1h 30m)</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>ANGELINI (1h 30m)</t>
-        </is>
-      </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h 30m)</t>
+          <t>SABATELLI (2h 30m)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (1h 30m)</t>
+          <t>SCHIAVONE (2h 30m)</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE (2h 30m)</t>
+          <t>MARANGI (1h 30m)</t>
         </is>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>MARANGI (2h 30m)</t>
+          <t>SIMEONE (1h 30m)</t>
         </is>
       </c>
       <c r="H24" s="4" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="I24" s="4" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J24" s="4" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="L24" s="4" t="inlineStr">
         <is>
-          <t>PEPE (1h) PALMISANO (0h 30m)</t>
+          <t>PEPE (2h)</t>
         </is>
       </c>
     </row>
@@ -1859,12 +1859,12 @@
       <c r="G25" s="4" t="inlineStr"/>
       <c r="H25" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO (1h)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>PALMISANO (3h)</t>
         </is>
       </c>
       <c r="J25" s="4" t="inlineStr">
@@ -1887,12 +1887,12 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
@@ -1907,12 +1907,12 @@
       </c>
       <c r="F26" s="5" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="H26" s="5" t="inlineStr">
@@ -1922,17 +1922,17 @@
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="J26" s="5" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="K26" s="5" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="L26" s="5" t="inlineStr"/>
@@ -1945,12 +1945,12 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>ANGELINI (2h)</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
@@ -1970,32 +1970,32 @@
       </c>
       <c r="G27" s="5" t="inlineStr">
         <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="H27" s="5" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="H27" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO (2h)</t>
-        </is>
-      </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>PEPE (2h)</t>
-        </is>
-      </c>
       <c r="J27" s="5" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="K27" s="5" t="inlineStr">
         <is>
-          <t>ZIZZI (2h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="L27" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -2012,52 +2012,52 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
+          <t>RUSSO (1h)</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE (3h)</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="H28" s="5" t="inlineStr">
+        <is>
+          <t>PALMISANO (3h)</t>
+        </is>
+      </c>
+      <c r="I28" s="5" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="D28" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E28" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="F28" s="5" t="inlineStr">
-        <is>
-          <t>SIMEONE (2h)</t>
-        </is>
-      </c>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="H28" s="5" t="inlineStr">
+      <c r="J28" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K28" s="5" t="inlineStr">
+        <is>
+          <t>CARDONE</t>
+        </is>
+      </c>
+      <c r="L28" s="5" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I28" s="5" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
-      <c r="J28" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K28" s="5" t="inlineStr">
-        <is>
-          <t>OSTUNI (1h)</t>
-        </is>
-      </c>
-      <c r="L28" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO (1h)</t>
         </is>
       </c>
     </row>
@@ -2069,39 +2069,39 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>ANGELINI (2h)</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H29" s="5" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="D29" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E29" s="5" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="F29" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI (1h)</t>
-        </is>
-      </c>
-      <c r="G29" s="5" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="H29" s="5" t="inlineStr">
-        <is>
-          <t>PEPE (2h)</t>
-        </is>
-      </c>
       <c r="I29" s="5" t="inlineStr">
         <is>
           <t>PALMISANO</t>
@@ -2109,17 +2109,17 @@
       </c>
       <c r="J29" s="5" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>ZIZZI (2h)</t>
         </is>
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="L29" s="5" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>PEPE (3h)</t>
         </is>
       </c>
     </row>
@@ -2131,37 +2131,37 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (3h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (3h)</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
           <t>CICCIMARRA (1h)</t>
         </is>
       </c>
-      <c r="D30" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (3h)</t>
-        </is>
-      </c>
-      <c r="E30" s="5" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
       <c r="F30" s="5" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>MARANGI (2h)</t>
         </is>
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="H30" s="5" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="I30" s="5" t="inlineStr">
@@ -2171,17 +2171,17 @@
       </c>
       <c r="J30" s="5" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>ZIZZI (1h)</t>
         </is>
       </c>
       <c r="L30" s="5" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
     </row>
@@ -2389,56 +2389,56 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr"/>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr"/>
       <c r="I2" s="1" t="inlineStr">
         <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
           <t>4A (1h)</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr"/>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="K2" s="1" t="inlineStr"/>
       <c r="L2" s="1" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="M2" s="1" t="inlineStr"/>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>5A (1h)</t>
         </is>
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
     </row>
@@ -2451,7 +2451,7 @@
       <c r="B3" s="1" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>1B (2h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -2461,30 +2461,30 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2B (2h)</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr"/>
       <c r="I3" s="1" t="inlineStr">
         <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
           <t>4B (1h)</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
           <t>5B</t>
@@ -2492,23 +2492,23 @@
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>1A (2h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="M3" s="1" t="inlineStr"/>
       <c r="N3" s="1" t="inlineStr">
         <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
           <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="O3" s="1" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
-      <c r="P3" s="1" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
         </is>
       </c>
     </row>
@@ -2520,55 +2520,55 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
+          <t>COPERTURA (0h 30m)</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>5A (3h)</t>
+          <t>5A (2h)</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (0h 30m)</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>2B (2h)</t>
+          <t>2A (2h)</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr"/>
       <c r="I4" s="1" t="inlineStr"/>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
+      <c r="J4" s="1" t="inlineStr"/>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
-      <c r="M4" s="1" t="inlineStr"/>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="M4" s="1" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
       <c r="N4" s="1" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="O4" s="1" t="inlineStr">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="P4" s="1" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
     </row>
@@ -2590,63 +2590,63 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
           <t>1B (2h)</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>1A (2h)</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr">
         <is>
+          <t>COPERTURA (2h)</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
+          <t>3A (3h)</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
           <t>3B (1h)</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
       <c r="I5" s="1" t="inlineStr"/>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>4A (3h)</t>
-        </is>
-      </c>
+      <c r="J5" s="1" t="inlineStr"/>
       <c r="K5" s="1" t="inlineStr">
         <is>
+          <t>5B (3h)</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr"/>
+      <c r="M5" s="1" t="inlineStr">
+        <is>
           <t>5A (1h)</t>
         </is>
       </c>
-      <c r="L5" s="1" t="inlineStr"/>
-      <c r="M5" s="1" t="inlineStr"/>
       <c r="N5" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>4B (2h)</t>
         </is>
       </c>
       <c r="O5" s="1" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="P5" s="1" t="inlineStr"/>
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="P5" s="1" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2656,63 +2656,63 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
+          <t>1B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
           <t>1A (1h 30m)</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>1B (1h 30m)</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="D6" s="1" t="inlineStr"/>
       <c r="E6" s="1" t="inlineStr">
         <is>
+          <t>2A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
           <t>2B (2h 30m)</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>2A (2h 30m)</t>
-        </is>
-      </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
+          <t>3B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
           <t>3A (1h 30m)</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>3B (1h 30m)</t>
-        </is>
-      </c>
       <c r="I6" s="1" t="inlineStr"/>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr"/>
+      <c r="J6" s="1" t="inlineStr"/>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="L6" s="1" t="inlineStr"/>
       <c r="M6" s="1" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="P6" s="1" t="inlineStr"/>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="P6" s="1" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2722,34 +2722,34 @@
       </c>
       <c r="B7" s="1" t="inlineStr"/>
       <c r="C7" s="1" t="inlineStr"/>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>5B (3h)</t>
-        </is>
-      </c>
+      <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr"/>
       <c r="G7" s="1" t="inlineStr"/>
       <c r="H7" s="1" t="inlineStr"/>
       <c r="I7" s="1" t="inlineStr"/>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>4B (2h)</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr"/>
+      <c r="J7" s="1" t="inlineStr"/>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>5A (2h)</t>
+        </is>
+      </c>
       <c r="L7" s="1" t="inlineStr"/>
       <c r="M7" s="1" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="O7" s="1" t="inlineStr"/>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="O7" s="1" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
       <c r="P7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
@@ -2760,12 +2760,12 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -2773,16 +2773,16 @@
           <t>5A</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
+      <c r="E8" s="2" t="inlineStr"/>
       <c r="F8" s="2" t="inlineStr"/>
-      <c r="G8" s="2" t="inlineStr"/>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>3B (1h)</t>
+        </is>
+      </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="L8" s="2" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="M8" s="2" t="inlineStr"/>
@@ -2807,12 +2807,12 @@
           <t>4B</t>
         </is>
       </c>
-      <c r="O8" s="2" t="inlineStr"/>
-      <c r="P8" s="2" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
+      <c r="O8" s="2" t="inlineStr">
+        <is>
+          <t>2B (1h)</t>
+        </is>
+      </c>
+      <c r="P8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -2822,33 +2822,33 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr"/>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="inlineStr"/>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3A (2h)</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
@@ -2859,12 +2859,12 @@
       <c r="J9" s="2" t="inlineStr"/>
       <c r="K9" s="2" t="inlineStr">
         <is>
-          <t>5B (2h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2A (2h)</t>
         </is>
       </c>
       <c r="M9" s="2" t="inlineStr"/>
@@ -2873,12 +2873,12 @@
           <t>4B (2h)</t>
         </is>
       </c>
-      <c r="O9" s="2" t="inlineStr"/>
-      <c r="P9" s="2" t="inlineStr">
+      <c r="O9" s="2" t="inlineStr">
         <is>
           <t>3B (1h)</t>
         </is>
       </c>
+      <c r="P9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -2888,61 +2888,61 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>1B (2h)</t>
+          <t>1A (3h)</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>1B (3h)</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5A (3h)</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>COPERTURA (2h)</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr"/>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B (3h)</t>
         </is>
       </c>
       <c r="L10" s="2" t="inlineStr"/>
       <c r="M10" s="2" t="inlineStr"/>
       <c r="N10" s="2" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="O10" s="2" t="inlineStr"/>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
     </row>
@@ -2954,65 +2954,65 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>2A (2h)</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>2B (3h)</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>3A (1h)</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>3B (2h)</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr"/>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>2B (2h)</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>2A (2h)</t>
-        </is>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
+      <c r="J11" s="2" t="inlineStr">
         <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>4B (2h)</t>
-        </is>
-      </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
       <c r="K11" s="2" t="inlineStr">
         <is>
           <t>5A</t>
         </is>
       </c>
       <c r="L11" s="2" t="inlineStr"/>
-      <c r="M11" s="2" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
+      <c r="M11" s="2" t="inlineStr"/>
       <c r="N11" s="2" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>4A (2h)</t>
         </is>
       </c>
       <c r="O11" s="2" t="inlineStr"/>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>1B (1h 30m)</t>
+          <t>1B (2h 30m)</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
@@ -3032,36 +3032,40 @@
           <t>1A (2h 30m)</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
+          <t>2B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
           <t>2A (1h 30m)</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>2B (1h 30m)</t>
-        </is>
-      </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
+          <t>3B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
           <t>3A (1h 30m)</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>3B (2h 30m)</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>COPERTURA (0h 30m)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
-          <t>5A (3h)</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="L12" s="2" t="inlineStr"/>
@@ -3075,14 +3079,10 @@
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="O12" s="2" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
+      <c r="O12" s="2" t="inlineStr"/>
       <c r="P12" s="2" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>COPERTURA (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -3094,7 +3094,11 @@
       </c>
       <c r="B13" s="2" t="inlineStr"/>
       <c r="C13" s="2" t="inlineStr"/>
-      <c r="D13" s="2" t="inlineStr"/>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>5B (3h)</t>
+        </is>
+      </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="2" t="inlineStr"/>
       <c r="G13" s="2" t="inlineStr"/>
@@ -3105,23 +3109,19 @@
           <t>4B (1h)</t>
         </is>
       </c>
-      <c r="K13" s="2" t="inlineStr"/>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>5A (3h)</t>
+        </is>
+      </c>
       <c r="L13" s="2" t="inlineStr"/>
       <c r="M13" s="2" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="N13" s="2" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="O13" s="2" t="inlineStr">
-        <is>
           <t>4A (1h)</t>
         </is>
       </c>
+      <c r="N13" s="2" t="inlineStr"/>
+      <c r="O13" s="2" t="inlineStr"/>
       <c r="P13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
@@ -3130,59 +3130,59 @@
           <t>MER1</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
+      <c r="B14" s="3" t="inlineStr"/>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr"/>
-      <c r="E14" s="3" t="inlineStr"/>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
       <c r="F14" s="3" t="inlineStr"/>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="H14" s="3" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr"/>
       <c r="I14" s="3" t="inlineStr">
         <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J14" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
       <c r="K14" s="3" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="L14" s="3" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="M14" s="3" t="inlineStr"/>
       <c r="N14" s="3" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="O14" s="3" t="inlineStr"/>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
       <c r="P14" s="3" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
     </row>
@@ -3192,20 +3192,20 @@
           <t>MER2</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>1B (2h)</t>
-        </is>
-      </c>
+      <c r="B15" s="3" t="inlineStr"/>
       <c r="C15" s="3" t="inlineStr">
         <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -3215,44 +3215,44 @@
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
+          <t>3B (2h)</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr"/>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="K15" s="3" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5A (1h)</t>
         </is>
       </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="M15" s="3" t="inlineStr"/>
       <c r="N15" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="O15" s="3" t="inlineStr"/>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="O15" s="3" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
       <c r="P15" s="3" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
     </row>
@@ -3264,14 +3264,14 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
+          <t>COPERTURA (0h 30m)</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (1h 30m)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
@@ -3289,40 +3289,40 @@
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>4B (3h)</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
         <is>
-          <t>4B (3h)</t>
+          <t>4A (3h)</t>
         </is>
       </c>
       <c r="K16" s="3" t="inlineStr"/>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
+      <c r="L16" s="3" t="inlineStr"/>
       <c r="M16" s="3" t="inlineStr"/>
       <c r="N16" s="3" t="inlineStr">
         <is>
+          <t>3A (2h)</t>
+        </is>
+      </c>
+      <c r="O16" s="3" t="inlineStr">
+        <is>
           <t>5A</t>
         </is>
       </c>
-      <c r="O16" s="3" t="inlineStr"/>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
     </row>
@@ -3334,61 +3334,61 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A (2h)</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5B (3h)</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>2A (2h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>3A (3h)</t>
+          <t>COPERTURA (2h)</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>3B (3h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K17" s="3" t="inlineStr"/>
       <c r="L17" s="3" t="inlineStr"/>
       <c r="M17" s="3" t="inlineStr"/>
-      <c r="N17" s="3" t="inlineStr">
-        <is>
-          <t>5A (3h)</t>
-        </is>
-      </c>
-      <c r="O17" s="3" t="inlineStr"/>
+      <c r="N17" s="3" t="inlineStr"/>
+      <c r="O17" s="3" t="inlineStr">
+        <is>
+          <t>5A (2h)</t>
+        </is>
+      </c>
       <c r="P17" s="3" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -3400,63 +3400,63 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>1A (3h 30m)</t>
+          <t>1A (1h 30m)</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>1B (3h 30m)</t>
+          <t>1B (1h 30m)</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2A (1h 30m)</t>
+          <t>2B (3h 30m)</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>2B (1h 30m)</t>
+          <t>2A (3h 30m)</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
+          <t>3A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
           <t>3B (1h 30m)</t>
         </is>
       </c>
-      <c r="H18" s="3" t="inlineStr">
-        <is>
-          <t>3A (1h 30m)</t>
-        </is>
-      </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (3h)</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr"/>
       <c r="L18" s="3" t="inlineStr"/>
       <c r="M18" s="3" t="inlineStr"/>
-      <c r="N18" s="3" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
+      <c r="N18" s="3" t="inlineStr"/>
       <c r="O18" s="3" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="P18" s="3" t="inlineStr"/>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="P18" s="3" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -3468,7 +3468,7 @@
       <c r="C19" s="3" t="inlineStr"/>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>5A (2h)</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
@@ -3477,12 +3477,12 @@
       <c r="H19" s="3" t="inlineStr"/>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>4A (3h)</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>4A (3h)</t>
+          <t>4B (3h)</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr"/>
@@ -3491,7 +3491,7 @@
       <c r="N19" s="3" t="inlineStr"/>
       <c r="O19" s="3" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5B (2h)</t>
         </is>
       </c>
       <c r="P19" s="3" t="inlineStr"/>
@@ -3502,7 +3502,11 @@
           <t>GIO1</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr"/>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
       <c r="C20" s="4" t="inlineStr"/>
       <c r="D20" s="4" t="inlineStr">
         <is>
@@ -3511,50 +3515,46 @@
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr"/>
-      <c r="G20" s="4" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
+      <c r="G20" s="4" t="inlineStr"/>
       <c r="H20" s="4" t="inlineStr">
         <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I20" s="4" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J20" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L20" s="4" t="inlineStr">
+        <is>
+          <t>2B (1h)</t>
+        </is>
+      </c>
+      <c r="M20" s="4" t="inlineStr"/>
+      <c r="N20" s="4" t="inlineStr"/>
+      <c r="O20" s="4" t="inlineStr">
+        <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="P20" s="4" t="inlineStr">
+        <is>
           <t>3A (1h)</t>
-        </is>
-      </c>
-      <c r="I20" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="J20" s="4" t="inlineStr"/>
-      <c r="K20" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L20" s="4" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="M20" s="4" t="inlineStr"/>
-      <c r="N20" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O20" s="4" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
-      <c r="P20" s="4" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
         </is>
       </c>
     </row>
@@ -3564,7 +3564,11 @@
           <t>GIO2</t>
         </is>
       </c>
-      <c r="B21" s="4" t="inlineStr"/>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="4" t="inlineStr">
         <is>
@@ -3573,54 +3577,50 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G21" s="4" t="inlineStr">
+          <t>2B (1h)</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr"/>
+      <c r="H21" s="4" t="inlineStr">
+        <is>
+          <t>3B (2h)</t>
+        </is>
+      </c>
+      <c r="I21" s="4" t="inlineStr">
+        <is>
+          <t>4B (2h)</t>
+        </is>
+      </c>
+      <c r="J21" s="4" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
+      <c r="K21" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L21" s="4" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="M21" s="4" t="inlineStr"/>
+      <c r="N21" s="4" t="inlineStr"/>
+      <c r="O21" s="4" t="inlineStr">
         <is>
           <t>3A (1h)</t>
         </is>
       </c>
-      <c r="H21" s="4" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
-        <is>
-          <t>4B (2h)</t>
-        </is>
-      </c>
-      <c r="J21" s="4" t="inlineStr"/>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L21" s="4" t="inlineStr">
-        <is>
-          <t>1B (2h)</t>
-        </is>
-      </c>
-      <c r="M21" s="4" t="inlineStr"/>
-      <c r="N21" s="4" t="inlineStr">
-        <is>
-          <t>4A (2h)</t>
-        </is>
-      </c>
-      <c r="O21" s="4" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
       <c r="P21" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
     </row>
@@ -3630,12 +3630,12 @@
           <t>GIO3</t>
         </is>
       </c>
-      <c r="B22" s="4" t="inlineStr"/>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr"/>
       <c r="D22" s="4" t="inlineStr">
         <is>
           <t>5B (3h)</t>
@@ -3643,50 +3643,50 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2A (3h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="G22" s="4" t="inlineStr">
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr"/>
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
         <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="H22" s="4" t="inlineStr">
-        <is>
-          <t>3B (2h)</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
       <c r="K22" s="4" t="inlineStr">
         <is>
           <t>5A (3h)</t>
         </is>
       </c>
-      <c r="L22" s="4" t="inlineStr"/>
+      <c r="L22" s="4" t="inlineStr">
+        <is>
+          <t>1A (2h)</t>
+        </is>
+      </c>
       <c r="M22" s="4" t="inlineStr"/>
       <c r="N22" s="4" t="inlineStr"/>
       <c r="O22" s="4" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="P22" s="4" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -3698,14 +3698,14 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
+          <t>1B (3h)</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
           <t>1A (1h)</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
           <t>5A</t>
@@ -3713,22 +3713,22 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>2B (3h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3A (2h)</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
@@ -3738,7 +3738,7 @@
       </c>
       <c r="J23" s="4" t="inlineStr">
         <is>
-          <t>4B (2h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K23" s="4" t="inlineStr">
@@ -3748,12 +3748,12 @@
       </c>
       <c r="L23" s="4" t="inlineStr"/>
       <c r="M23" s="4" t="inlineStr"/>
-      <c r="N23" s="4" t="inlineStr"/>
-      <c r="O23" s="4" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
+      <c r="N23" s="4" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="O23" s="4" t="inlineStr"/>
       <c r="P23" s="4" t="inlineStr">
         <is>
           <t>4A (1h)</t>
@@ -3768,14 +3768,14 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
+          <t>1A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
           <t>1B (1h 30m)</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>1A (1h 30m)</t>
-        </is>
-      </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
           <t>5A</t>
@@ -3783,22 +3783,22 @@
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>2B (1h 30m)</t>
+          <t>2A (2h 30m)</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>2A (1h 30m)</t>
+          <t>2B (2h 30m)</t>
         </is>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>3B (2h 30m)</t>
+          <t>3A (1h 30m)</t>
         </is>
       </c>
       <c r="H24" s="4" t="inlineStr">
         <is>
-          <t>3A (2h 30m)</t>
+          <t>3B (1h 30m)</t>
         </is>
       </c>
       <c r="I24" s="4" t="inlineStr">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="J24" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (0h 30m)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K24" s="4" t="inlineStr">
@@ -3818,15 +3818,15 @@
       </c>
       <c r="L24" s="4" t="inlineStr"/>
       <c r="M24" s="4" t="inlineStr"/>
-      <c r="N24" s="4" t="inlineStr"/>
-      <c r="O24" s="4" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
+      <c r="N24" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="O24" s="4" t="inlineStr"/>
       <c r="P24" s="4" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>COPERTURA (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -3850,7 +3850,7 @@
       <c r="I25" s="4" t="inlineStr"/>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>4B (3h)</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
@@ -3860,12 +3860,12 @@
       </c>
       <c r="L25" s="4" t="inlineStr"/>
       <c r="M25" s="4" t="inlineStr"/>
-      <c r="N25" s="4" t="inlineStr"/>
-      <c r="O25" s="4" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
+      <c r="N25" s="4" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
+      <c r="O25" s="4" t="inlineStr"/>
       <c r="P25" s="4" t="inlineStr"/>
     </row>
     <row r="26">
@@ -3876,17 +3876,17 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
@@ -3898,12 +3898,12 @@
       <c r="G26" s="5" t="inlineStr"/>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="J26" s="5" t="inlineStr">
@@ -3911,19 +3911,19 @@
           <t>4A</t>
         </is>
       </c>
-      <c r="K26" s="5" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
+      <c r="K26" s="5" t="inlineStr"/>
       <c r="L26" s="5" t="inlineStr"/>
-      <c r="M26" s="5" t="inlineStr"/>
-      <c r="N26" s="5" t="inlineStr"/>
-      <c r="O26" s="5" t="inlineStr">
-        <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
+      <c r="M26" s="5" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="N26" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="O26" s="5" t="inlineStr"/>
       <c r="P26" s="5" t="inlineStr">
         <is>
           <t>2A (1h)</t>
@@ -3938,17 +3938,17 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>1B (2h)</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1A (2h)</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
+          <t>5A (1h)</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
@@ -3969,30 +3969,30 @@
       </c>
       <c r="I27" s="5" t="inlineStr">
         <is>
-          <t>4B (2h)</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="J27" s="5" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
-        </is>
-      </c>
-      <c r="K27" s="5" t="inlineStr">
-        <is>
-          <t>5B (2h)</t>
-        </is>
-      </c>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="K27" s="5" t="inlineStr"/>
       <c r="L27" s="5" t="inlineStr"/>
-      <c r="M27" s="5" t="inlineStr"/>
-      <c r="N27" s="5" t="inlineStr"/>
-      <c r="O27" s="5" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
+      <c r="M27" s="5" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="N27" s="5" t="inlineStr">
+        <is>
+          <t>3B (2h)</t>
+        </is>
+      </c>
+      <c r="O27" s="5" t="inlineStr"/>
       <c r="P27" s="5" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -4007,32 +4007,36 @@
           <t>1A</t>
         </is>
       </c>
-      <c r="C28" s="5" t="inlineStr"/>
-      <c r="D28" s="5" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr"/>
       <c r="E28" s="5" t="inlineStr"/>
       <c r="F28" s="5" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="G28" s="5" t="inlineStr"/>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>3B (1h)</t>
+        </is>
+      </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>3A (3h)</t>
         </is>
       </c>
       <c r="I28" s="5" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="J28" s="5" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>4A (3h)</t>
         </is>
       </c>
       <c r="K28" s="5" t="inlineStr">
@@ -4041,19 +4045,15 @@
         </is>
       </c>
       <c r="L28" s="5" t="inlineStr"/>
-      <c r="M28" s="5" t="inlineStr">
+      <c r="M28" s="5" t="inlineStr"/>
+      <c r="N28" s="5" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="O28" s="5" t="inlineStr">
         <is>
           <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="N28" s="5" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="O28" s="5" t="inlineStr">
-        <is>
-          <t>1B (1h)</t>
         </is>
       </c>
       <c r="P28" s="5" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1A (2h)</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr"/>
@@ -4083,13 +4083,17 @@
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
-        </is>
-      </c>
-      <c r="H29" s="5" t="inlineStr"/>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H29" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
       <c r="I29" s="5" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>COPERTURA (3h)</t>
         </is>
       </c>
       <c r="J29" s="5" t="inlineStr">
@@ -4099,32 +4103,28 @@
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5A (2h)</t>
         </is>
       </c>
       <c r="L29" s="5" t="inlineStr">
         <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="M29" s="5" t="inlineStr"/>
+      <c r="N29" s="5" t="inlineStr">
+        <is>
+          <t>5B (2h)</t>
+        </is>
+      </c>
+      <c r="O29" s="5" t="inlineStr">
+        <is>
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="M29" s="5" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="N29" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="O29" s="5" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
       <c r="P29" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
     </row>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>1A (3h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr"/>
@@ -4149,13 +4149,17 @@
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="H30" s="5" t="inlineStr"/>
+          <t>3A (2h)</t>
+        </is>
+      </c>
+      <c r="H30" s="5" t="inlineStr">
+        <is>
+          <t>3B (2h)</t>
+        </is>
+      </c>
       <c r="I30" s="5" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
       <c r="J30" s="5" t="inlineStr">
@@ -4165,32 +4169,28 @@
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>5A (3h)</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="L30" s="5" t="inlineStr">
         <is>
+          <t>2B (1h)</t>
+        </is>
+      </c>
+      <c r="M30" s="5" t="inlineStr"/>
+      <c r="N30" s="5" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="O30" s="5" t="inlineStr">
+        <is>
           <t>1B (1h)</t>
         </is>
       </c>
-      <c r="M30" s="5" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="N30" s="5" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="O30" s="5" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
       <c r="P30" s="5" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add validation and handling for specific teacher assignments in scheduling
- Implemented validation for 'ASSEGNAZIONE_DOCENTI_SPECIFICHE' in the configuration.
- Enhanced the schedule generation logic to accommodate specific assignments for teachers.
- Updated the configuration loading and saving functions to handle the new assignment format.
- Modified the UI to allow input of specific assignments for teachers, including validation checks.
</commit_message>
<xml_diff>
--- a/orario_settimanale.xlsx
+++ b/orario_settimanale.xlsx
@@ -527,52 +527,52 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>MARANGI (1h)</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI (1h)</t>
-        </is>
-      </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
+          <t>PEPE (1h)</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
           <t>PALMISANO (1h)</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>PEPE (1h)</t>
-        </is>
-      </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="L2" s="1" t="inlineStr"/>
@@ -585,57 +585,57 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI (2h)</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>RUSSO (1h)</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (1h)</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>SABATELLI (2h)</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI (2h)</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
+          <t>MOTORIA (1h)</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
           <t>PEPE (1h)</t>
         </is>
       </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>PALMISANO (1h)</t>
-        </is>
-      </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (1h) RUSSO (1h)</t>
+          <t>SAVINO (1h) PALMISANO (1h)</t>
         </is>
       </c>
     </row>
@@ -647,27 +647,27 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -677,27 +677,27 @@
       </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
           <t>MOTORIA (1h)</t>
         </is>
       </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
-        </is>
-      </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>ZIZZI (3h)</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>RUSSO (1h) MARANGI (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -709,57 +709,57 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>RUSSO (1h)</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>SIMEONE (1h)</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PALMISANO (2h)</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>MOTORIA (1h)</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr">
+        <is>
           <t>ANGELINI (1h)</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>RUSSO (2h)</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>MARANGI (3h)</t>
-        </is>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>SIMEONE (1h)</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>CARDONE (2h)</t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>ZIZZI (3h)</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
-        <is>
-          <t>SABATELLI (2h)</t>
         </is>
       </c>
     </row>
@@ -771,22 +771,22 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
+          <t>ANGELINI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
           <t>RUSSO (1h 30m)</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>ANGELINI (1h 30m)</t>
-        </is>
-      </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>SABATELLI (1h 30m)</t>
+          <t>SABATELLI (3h 30m)</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h 30m)</t>
+          <t>SCHIAVONE (3h 30m)</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
@@ -801,27 +801,27 @@
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>ZIZZI (2h)</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr">
         <is>
-          <t>CARDONE (1h)</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
     </row>
@@ -839,22 +839,22 @@
       <c r="G7" s="1" t="inlineStr"/>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>LEO (2h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>OSTUNI (2h)</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
           <t>MOTORIA (1h)</t>
-        </is>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>ZIZZI (2h)</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr"/>
@@ -867,17 +867,17 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>RUSSO (1h)</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
@@ -887,32 +887,32 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
           <t>PEPE</t>
         </is>
       </c>
-      <c r="I8" s="2" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
-        </is>
-      </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
+          <t>ZIZZI</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
           <t>OSTUNI</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="inlineStr">
-        <is>
-          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L8" s="2" t="inlineStr"/>
@@ -925,52 +925,52 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>CICCIMARRA (2h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SCHIAVONE (1h)</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>SIMEONE (2h)</t>
+          <t>SIMEONE (1h)</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>PEPE (2h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>ZIZZI (2h)</t>
         </is>
       </c>
       <c r="K9" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI (2h)</t>
         </is>
       </c>
       <c r="L9" s="2" t="inlineStr">
@@ -987,24 +987,24 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI (3h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (3h)</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
           <t>SABATELLI</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
           <t>SAVINO (1h)</t>
@@ -1017,22 +1017,22 @@
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>CARDONE</t>
+          <t>PALMISANO (3h)</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>PEPE (3h)</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI (3h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="L10" s="2" t="inlineStr">
@@ -1049,27 +1049,27 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>RUSSO (3h)</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
+          <t>SCHIAVONE (2h)</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
           <t>SABATELLI (2h)</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (3h)</t>
-        </is>
-      </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
@@ -1079,27 +1079,27 @@
       </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="I11" s="2" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="K11" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>PALMISANO (1h) PEPE (1h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
     </row>
@@ -1111,24 +1111,24 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>RUSSO (2h 30m)</t>
+          <t>CICCIMARRA (1h 30m)</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>ANGELINI (2h 30m)</t>
+          <t>ANGELINI (1h 30m)</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
+          <t>SABATELLI (1h 30m)</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
           <t>SCHIAVONE (1h 30m)</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h 30m)</t>
-        </is>
-      </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
           <t>SIMEONE (1h 30m)</t>
@@ -1141,27 +1141,27 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>PALMISANO (1h)</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>PALMISANO (2h)</t>
         </is>
       </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
+          <t>OSTUNI</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
         </is>
       </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>OSTUNI</t>
-        </is>
-      </c>
       <c r="L12" s="2" t="inlineStr">
         <is>
-          <t>CARDONE (1h) SAVINO (0h 30m)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
     </row>
@@ -1184,17 +1184,17 @@
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
-          <t>PALMISANO (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>ZIZZI (3h)</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="K13" s="2" t="inlineStr">
         <is>
-          <t>OSTUNI (3h)</t>
+          <t>ZIZZI (2h)</t>
         </is>
       </c>
       <c r="L13" s="2" t="inlineStr"/>
@@ -1207,47 +1207,47 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
+          <t>RUSSO</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>SABATELLI (1h)</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>CARDONE</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
           <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>RUSSO (1h)</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI</t>
-        </is>
-      </c>
-      <c r="H14" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="J14" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE (1h)</t>
         </is>
       </c>
       <c r="K14" s="3" t="inlineStr">
@@ -1265,32 +1265,32 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
+          <t>RUSSO</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>ANGELINI</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (1h)</t>
-        </is>
-      </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>CARDONE</t>
+          <t>MARANGI (2h)</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>MARANGI (2h)</t>
+          <t>SIMEONE (2h)</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
@@ -1310,12 +1310,12 @@
       </c>
       <c r="K15" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI (1h) RUSSO (1h)</t>
+          <t>SABATELLI</t>
         </is>
       </c>
     </row>
@@ -1327,34 +1327,34 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>RUSSO (3h)</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
+          <t>ANGELINI (2h)</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (2h)</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>SCHIAVONE</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>SABATELLI</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>CARDONE (2h)</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>SIMEONE (1h)</t>
-        </is>
-      </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
           <t>PALMISANO (3h)</t>
@@ -1362,22 +1362,22 @@
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>PEPE (3h)</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>OSTUNI (1h)</t>
         </is>
       </c>
       <c r="K16" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI</t>
+          <t>LEO (2h)</t>
         </is>
       </c>
       <c r="L16" s="3" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>SABATELLI (2h)</t>
         </is>
       </c>
     </row>
@@ -1389,57 +1389,57 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>RUSSO (2h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI (1h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SABATELLI (1h)</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>SCHIAVONE (1h)</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE (1h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="H17" s="3" t="inlineStr">
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>PALMISANO</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>CARDONE</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>OSTUNI</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
         <is>
           <t>PEPE</t>
-        </is>
-      </c>
-      <c r="I17" s="3" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="J17" s="3" t="inlineStr">
-        <is>
-          <t>LEO (2h)</t>
-        </is>
-      </c>
-      <c r="K17" s="3" t="inlineStr">
-        <is>
-          <t>OSTUNI (3h)</t>
-        </is>
-      </c>
-      <c r="L17" s="3" t="inlineStr">
-        <is>
-          <t>MARANGI (2h)</t>
         </is>
       </c>
     </row>
@@ -1451,37 +1451,37 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>ANGELINI (1h 30m)</t>
+          <t>ANGELINI (2h 30m)</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>RUSSO (1h 30m)</t>
+          <t>RUSSO (2h 30m)</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>SCHIAVONE (3h 30m)</t>
+          <t>SCHIAVONE (1h 30m)</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>SABATELLI (3h 30m)</t>
+          <t>SABATELLI (1h 30m)</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>MARANGI (1h 30m)</t>
+          <t>SIMEONE (3h 30m)</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>SIMEONE (1h 30m)</t>
+          <t>MARANGI (2h 30m)</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
@@ -1491,17 +1491,17 @@
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
+          <t>CARDONE</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
           <t>OSTUNI</t>
         </is>
       </c>
-      <c r="K18" s="3" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
       <c r="L18" s="3" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PEPE (2h)</t>
         </is>
       </c>
     </row>
@@ -1519,7 +1519,7 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>PEPE (3h)</t>
+          <t>PEPE (1h)</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -1529,12 +1529,12 @@
       </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>OSTUNI (2h)</t>
+          <t>CARDONE (3h)</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr">
         <is>
-          <t>LEO (2h)</t>
+          <t>OSTUNI (3h)</t>
         </is>
       </c>
       <c r="L19" s="3" t="inlineStr"/>
@@ -1547,37 +1547,37 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
+          <t>RUSSO</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
           <t>ANGELINI (1h)</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="inlineStr">
+        <is>
+          <t>SIMEONE (1h)</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
         <is>
           <t>LEO (1h)</t>
         </is>
       </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="G20" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PALMISANO (1h)</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -1605,37 +1605,37 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>CICCIMARRA</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
+          <t>SABATELLI</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (1h)</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE (2h)</t>
+          <t>SIMEONE</t>
         </is>
       </c>
       <c r="H21" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO (2h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="I21" s="4" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L21" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
     </row>
@@ -1667,57 +1667,57 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>CICCIMARRA (2h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE (1h)</t>
+          <t>SABATELLI (2h)</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (1h)</t>
+          <t>SCHIAVONE (2h)</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>CARDONE (2h)</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
         <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="H22" s="4" t="inlineStr">
+      <c r="J22" s="4" t="inlineStr">
+        <is>
+          <t>ZIZZI (3h)</t>
+        </is>
+      </c>
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>OSTUNI (3h)</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
         <is>
           <t>PEPE (1h)</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>ZIZZI (3h)</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>OSTUNI (3h)</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>PALMISANO (1h)</t>
         </is>
       </c>
     </row>
@@ -1729,37 +1729,37 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>ANGELINI (1h)</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>ANGELINI (3h)</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI</t>
+          <t>SCHIAVONE</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>SIMEONE (2h)</t>
+          <t>MARANGI (2h)</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>MARANGI (1h)</t>
+          <t>SIMEONE (3h)</t>
         </is>
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
@@ -1779,7 +1779,7 @@
       </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>SABATELLI (1h) CARDONE (1h)</t>
         </is>
       </c>
     </row>
@@ -1791,42 +1791,42 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
           <t>ANGELINI (1h 30m)</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>RUSSO (1h 30m)</t>
-        </is>
-      </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>SABATELLI (2h 30m)</t>
+          <t>SCHIAVONE (2h 30m)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>SCHIAVONE (2h 30m)</t>
+          <t>SABATELLI (1h 30m)</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
+          <t>SIMEONE (1h 30m)</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
           <t>MARANGI (1h 30m)</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>SIMEONE (1h 30m)</t>
-        </is>
-      </c>
       <c r="H24" s="4" t="inlineStr">
         <is>
-          <t>CARDONE</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I24" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PALMISANO (2h)</t>
         </is>
       </c>
       <c r="J24" s="4" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="L24" s="4" t="inlineStr">
         <is>
-          <t>PEPE (2h)</t>
+          <t>SAVINO (1h) RUSSO (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -1859,12 +1859,12 @@
       <c r="G25" s="4" t="inlineStr"/>
       <c r="H25" s="4" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>PEPE (3h)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
         <is>
-          <t>PALMISANO (3h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="J25" s="4" t="inlineStr">
@@ -1887,17 +1887,17 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>RUSSO</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>CICCIMARRA (1h)</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>LEO (1h)</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
@@ -1907,32 +1907,32 @@
       </c>
       <c r="F26" s="5" t="inlineStr">
         <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
           <t>SIMEONE</t>
         </is>
       </c>
-      <c r="G26" s="5" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
-        </is>
-      </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
-          <t>PEPE (1h)</t>
+          <t>MOTORIA (1h)</t>
         </is>
       </c>
       <c r="J26" s="5" t="inlineStr">
         <is>
-          <t>MOTORIA (1h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="K26" s="5" t="inlineStr">
         <is>
-          <t>OSTUNI (1h)</t>
+          <t>OSTUNI</t>
         </is>
       </c>
       <c r="L26" s="5" t="inlineStr"/>
@@ -1945,57 +1945,57 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>RUSSO (2h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (2h)</t>
+          <t>RUSSO</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>MARANGI</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>SIMEONE</t>
+        </is>
+      </c>
+      <c r="H27" s="5" t="inlineStr">
+        <is>
+          <t>PEPE (2h)</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>SAVINO (1h)</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI (2h)</t>
+        </is>
+      </c>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>OSTUNI (2h)</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
           <t>SABATELLI (1h)</t>
-        </is>
-      </c>
-      <c r="E27" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (1h)</t>
-        </is>
-      </c>
-      <c r="F27" s="5" t="inlineStr">
-        <is>
-          <t>SIMEONE</t>
-        </is>
-      </c>
-      <c r="G27" s="5" t="inlineStr">
-        <is>
-          <t>CARDONE (2h)</t>
-        </is>
-      </c>
-      <c r="H27" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO</t>
-        </is>
-      </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>SAVINO (1h)</t>
-        </is>
-      </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>OSTUNI (1h)</t>
-        </is>
-      </c>
-      <c r="K27" s="5" t="inlineStr">
-        <is>
-          <t>MOTORIA (1h)</t>
-        </is>
-      </c>
-      <c r="L27" s="5" t="inlineStr">
-        <is>
-          <t>PEPE</t>
         </is>
       </c>
     </row>
@@ -2007,52 +2007,52 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI</t>
+          <t>ANGELINI (2h)</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>RUSSO (1h)</t>
+          <t>RUSSO (2h)</t>
         </is>
       </c>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>SCHIAVONE</t>
+          <t>SABATELLI (1h)</t>
         </is>
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>SCHIAVONE (2h)</t>
         </is>
       </c>
       <c r="F28" s="5" t="inlineStr">
         <is>
+          <t>MARANGI (3h)</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
           <t>SIMEONE (3h)</t>
         </is>
       </c>
-      <c r="G28" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI (1h)</t>
-        </is>
-      </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
-          <t>PALMISANO (3h)</t>
+          <t>CARDONE</t>
         </is>
       </c>
       <c r="I28" s="5" t="inlineStr">
         <is>
-          <t>LEO (1h)</t>
+          <t>PALMISANO</t>
         </is>
       </c>
       <c r="J28" s="5" t="inlineStr">
         <is>
+          <t>OSTUNI</t>
+        </is>
+      </c>
+      <c r="K28" s="5" t="inlineStr">
+        <is>
           <t>ZIZZI</t>
-        </is>
-      </c>
-      <c r="K28" s="5" t="inlineStr">
-        <is>
-          <t>CARDONE</t>
         </is>
       </c>
       <c r="L28" s="5" t="inlineStr">
@@ -2069,12 +2069,12 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>ANGELINI (2h)</t>
+          <t>RUSSO (1h)</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>CICCIMARRA (1h)</t>
+          <t>ANGELINI</t>
         </is>
       </c>
       <c r="D29" s="5" t="inlineStr">
@@ -2089,37 +2089,37 @@
       </c>
       <c r="F29" s="5" t="inlineStr">
         <is>
-          <t>MARANGI</t>
+          <t>SIMEONE (1h)</t>
         </is>
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE</t>
+          <t>SAVINO (1h)</t>
         </is>
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
-          <t>SAVINO (1h)</t>
+          <t>CARDONE (2h)</t>
         </is>
       </c>
       <c r="I29" s="5" t="inlineStr">
         <is>
-          <t>PALMISANO</t>
+          <t>PALMISANO (2h)</t>
         </is>
       </c>
       <c r="J29" s="5" t="inlineStr">
         <is>
-          <t>ZIZZI (2h)</t>
+          <t>OSTUNI (2h)</t>
         </is>
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>CARDONE (2h)</t>
+          <t>ZIZZI</t>
         </is>
       </c>
       <c r="L29" s="5" t="inlineStr">
         <is>
-          <t>PEPE (3h)</t>
+          <t>PEPE (2h)</t>
         </is>
       </c>
     </row>
@@ -2131,57 +2131,57 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
+          <t>LEO (1h)</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>ANGELINI (2h)</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>SCHIAVONE (2h)</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
+          <t>CICCIMARRA (1h)</t>
+        </is>
+      </c>
+      <c r="F30" s="5" t="inlineStr">
+        <is>
           <t>SAVINO (1h)</t>
         </is>
       </c>
-      <c r="C30" s="5" t="inlineStr">
-        <is>
-          <t>LEO (1h)</t>
-        </is>
-      </c>
-      <c r="D30" s="5" t="inlineStr">
-        <is>
-          <t>SCHIAVONE (3h)</t>
-        </is>
-      </c>
-      <c r="E30" s="5" t="inlineStr">
-        <is>
-          <t>CICCIMARRA (1h)</t>
-        </is>
-      </c>
-      <c r="F30" s="5" t="inlineStr">
-        <is>
-          <t>MARANGI (2h)</t>
-        </is>
-      </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>SIMEONE (2h)</t>
+          <t>MARANGI (1h)</t>
         </is>
       </c>
       <c r="H30" s="5" t="inlineStr">
         <is>
+          <t>PALMISANO (1h)</t>
+        </is>
+      </c>
+      <c r="I30" s="5" t="inlineStr">
+        <is>
           <t>PEPE (1h)</t>
         </is>
       </c>
-      <c r="I30" s="5" t="inlineStr">
-        <is>
-          <t>PALMISANO (2h)</t>
-        </is>
-      </c>
       <c r="J30" s="5" t="inlineStr">
         <is>
+          <t>MOTORIA (1h)</t>
+        </is>
+      </c>
+      <c r="K30" s="5" t="inlineStr">
+        <is>
+          <t>ZIZZI (3h)</t>
+        </is>
+      </c>
+      <c r="L30" s="5" t="inlineStr">
+        <is>
           <t>CARDONE (1h)</t>
-        </is>
-      </c>
-      <c r="K30" s="5" t="inlineStr">
-        <is>
-          <t>ZIZZI (1h)</t>
-        </is>
-      </c>
-      <c r="L30" s="5" t="inlineStr">
-        <is>
-          <t>ANGELINI (1h)</t>
         </is>
       </c>
     </row>
@@ -2386,17 +2386,13 @@
           <t>LUN1</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr"/>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr"/>
+      <c r="D2" s="1" t="inlineStr"/>
       <c r="E2" s="1" t="inlineStr">
         <is>
           <t>2B</t>
@@ -2405,21 +2401,25 @@
       <c r="F2" s="1" t="inlineStr"/>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr"/>
       <c r="I2" s="1" t="inlineStr">
         <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
           <t>4B (1h)</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr"/>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="L2" s="1" t="inlineStr">
         <is>
           <t>2A (1h)</t>
@@ -2428,17 +2428,17 @@
       <c r="M2" s="1" t="inlineStr"/>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -2448,17 +2448,17 @@
           <t>LUN2</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr"/>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>1A (2h)</t>
+        </is>
+      </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr"/>
       <c r="E3" s="1" t="inlineStr">
         <is>
           <t>2B (2h)</t>
@@ -2466,49 +2466,53 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr"/>
       <c r="I3" s="1" t="inlineStr">
         <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>BUCO</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
           <t>4A (1h)</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
-      <c r="M3" s="1" t="inlineStr"/>
       <c r="N3" s="1" t="inlineStr">
         <is>
+          <t>5B (2h)</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>3A (1h)</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
           <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="O3" s="1" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
-      <c r="P3" s="1" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -2520,65 +2524,69 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
           <t>COPERTURA (0h 30m)</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>5A (2h)</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>2A (2h)</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>3A</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr"/>
       <c r="I4" s="1" t="inlineStr"/>
-      <c r="J4" s="1" t="inlineStr"/>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A (3h)</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
+          <t>BUCO (2h)</t>
+        </is>
+      </c>
+      <c r="M4" s="1" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="N4" s="1" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="O4" s="1" t="inlineStr">
+        <is>
+          <t>3B (1h)</t>
+        </is>
+      </c>
+      <c r="P4" s="1" t="inlineStr">
+        <is>
           <t>1A (1h)</t>
-        </is>
-      </c>
-      <c r="M4" s="1" t="inlineStr">
-        <is>
-          <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="N4" s="1" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="O4" s="1" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="P4" s="1" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
         </is>
       </c>
     </row>
@@ -2590,18 +2598,22 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
           <t>1A (1h)</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>1B (2h)</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr"/>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>BUCO (1h)</t>
+        </is>
+      </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
@@ -2611,7 +2623,7 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>3A (3h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -2620,13 +2632,21 @@
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr"/>
-      <c r="J5" s="1" t="inlineStr"/>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr"/>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr">
+        <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
       <c r="M5" s="1" t="inlineStr">
         <is>
           <t>5A (1h)</t>
@@ -2634,17 +2654,17 @@
       </c>
       <c r="N5" s="1" t="inlineStr">
         <is>
-          <t>4B (2h)</t>
+          <t>3A (2h)</t>
         </is>
       </c>
       <c r="O5" s="1" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>BUCO</t>
         </is>
       </c>
       <c r="P5" s="1" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
     </row>
@@ -2656,23 +2676,27 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
+          <t>1A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
           <t>1B (1h 30m)</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>1A (1h 30m)</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr"/>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>2A (1h 30m)</t>
+          <t>2A (3h 30m)</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>2B (2h 30m)</t>
+          <t>2B (3h 30m)</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
@@ -2686,31 +2710,35 @@
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr"/>
-      <c r="J6" s="1" t="inlineStr"/>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B (2h)</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr"/>
       <c r="M6" s="1" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>BUCO (2h)</t>
         </is>
       </c>
       <c r="P6" s="1" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
     </row>
@@ -2722,32 +2750,32 @@
       </c>
       <c r="B7" s="1" t="inlineStr"/>
       <c r="C7" s="1" t="inlineStr"/>
-      <c r="D7" s="1" t="inlineStr"/>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>5A (2h)</t>
+        </is>
+      </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr"/>
       <c r="G7" s="1" t="inlineStr"/>
       <c r="H7" s="1" t="inlineStr"/>
       <c r="I7" s="1" t="inlineStr"/>
       <c r="J7" s="1" t="inlineStr"/>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>5A (2h)</t>
-        </is>
-      </c>
+      <c r="K7" s="1" t="inlineStr"/>
       <c r="L7" s="1" t="inlineStr"/>
       <c r="M7" s="1" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>5B (1h)</t>
         </is>
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>4B (2h)</t>
         </is>
       </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
       <c r="P7" s="1" t="inlineStr"/>
@@ -2760,51 +2788,47 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1B (1h)</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr"/>
       <c r="F8" s="2" t="inlineStr"/>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
+          <t>3A (1h)</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr"/>
       <c r="I8" s="2" t="inlineStr">
         <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
           <t>4A</t>
         </is>
       </c>
-      <c r="J8" s="2" t="inlineStr"/>
       <c r="K8" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr"/>
       <c r="M8" s="2" t="inlineStr"/>
       <c r="N8" s="2" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="O8" s="2" t="inlineStr">
@@ -2812,7 +2836,11 @@
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="P8" s="2" t="inlineStr"/>
+      <c r="P8" s="2" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -2822,23 +2850,23 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B (2h)</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr"/>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
@@ -2848,37 +2876,41 @@
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
-        </is>
-      </c>
-      <c r="J9" s="2" t="inlineStr"/>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="K9" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>2A (2h)</t>
-        </is>
-      </c>
+          <t>5A (2h)</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr"/>
       <c r="M9" s="2" t="inlineStr"/>
       <c r="N9" s="2" t="inlineStr">
         <is>
-          <t>4B (2h)</t>
+          <t>3B (2h)</t>
         </is>
       </c>
       <c r="O9" s="2" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
-        </is>
-      </c>
-      <c r="P9" s="2" t="inlineStr"/>
+          <t>2A (1h)</t>
+        </is>
+      </c>
+      <c r="P9" s="2" t="inlineStr">
+        <is>
+          <t>BUCO (1h)</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -2888,32 +2920,32 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>1A (3h)</t>
+          <t>BUCO</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>1B (3h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>5A (3h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
@@ -2923,23 +2955,35 @@
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="J10" s="2" t="inlineStr"/>
+          <t>4B (3h)</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>4A (3h)</t>
+        </is>
+      </c>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr"/>
+          <t>BUCO</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
+        <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
       <c r="M10" s="2" t="inlineStr"/>
       <c r="N10" s="2" t="inlineStr">
         <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O10" s="2" t="inlineStr"/>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="O10" s="2" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
           <t>3A (1h)</t>
@@ -2954,65 +2998,77 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>BUCO (2h)</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1A (3h)</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
+          <t>2B (2h)</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
           <t>2A (2h)</t>
         </is>
       </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>2B (3h)</t>
-        </is>
-      </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
+          <t>COPERTURA (3h)</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>3B (2h)</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>BUCO (2h)</t>
+        </is>
+      </c>
+      <c r="L11" s="2" t="inlineStr">
+        <is>
+          <t>BUCO (1h)</t>
+        </is>
+      </c>
+      <c r="M11" s="2" t="inlineStr">
+        <is>
+          <t>5B (1h)</t>
+        </is>
+      </c>
+      <c r="N11" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="O11" s="2" t="inlineStr">
+        <is>
           <t>3A (1h)</t>
         </is>
       </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>3B (2h)</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L11" s="2" t="inlineStr"/>
-      <c r="M11" s="2" t="inlineStr"/>
-      <c r="N11" s="2" t="inlineStr">
-        <is>
-          <t>4A (2h)</t>
-        </is>
-      </c>
-      <c r="O11" s="2" t="inlineStr"/>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
     </row>
@@ -3024,27 +3080,27 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>1B (2h 30m)</t>
+          <t>1B (1h 30m)</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>1A (2h 30m)</t>
+          <t>COPERTURA (0h 30m)</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
+          <t>2A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
           <t>2B (1h 30m)</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>2A (1h 30m)</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
@@ -3060,29 +3116,37 @@
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr">
         <is>
+          <t>4B (2h)</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr">
+        <is>
+          <t>1A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="M12" s="2" t="inlineStr">
+        <is>
+          <t>BUCO (1h)</t>
+        </is>
+      </c>
+      <c r="N12" s="2" t="inlineStr">
+        <is>
+          <t>COPERTURA (2h)</t>
+        </is>
+      </c>
+      <c r="O12" s="2" t="inlineStr">
+        <is>
+          <t>BUCO (1h)</t>
+        </is>
+      </c>
+      <c r="P12" s="2" t="inlineStr">
+        <is>
           <t>4A (1h)</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L12" s="2" t="inlineStr"/>
-      <c r="M12" s="2" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="N12" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="O12" s="2" t="inlineStr"/>
-      <c r="P12" s="2" t="inlineStr">
-        <is>
-          <t>COPERTURA (0h 30m)</t>
         </is>
       </c>
     </row>
@@ -3096,7 +3160,7 @@
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
+          <t>5A (3h)</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
@@ -3104,14 +3168,10 @@
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="2" t="inlineStr"/>
       <c r="I13" s="2" t="inlineStr"/>
-      <c r="J13" s="2" t="inlineStr">
-        <is>
-          <t>4B (1h)</t>
-        </is>
-      </c>
+      <c r="J13" s="2" t="inlineStr"/>
       <c r="K13" s="2" t="inlineStr">
         <is>
-          <t>5A (3h)</t>
+          <t>5B (2h)</t>
         </is>
       </c>
       <c r="L13" s="2" t="inlineStr"/>
@@ -3121,7 +3181,11 @@
         </is>
       </c>
       <c r="N13" s="2" t="inlineStr"/>
-      <c r="O13" s="2" t="inlineStr"/>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
       <c r="P13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
@@ -3133,27 +3197,27 @@
       <c r="B14" s="3" t="inlineStr"/>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr"/>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr"/>
       <c r="G14" s="3" t="inlineStr">
         <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="H14" s="3" t="inlineStr"/>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
+      <c r="I14" s="3" t="inlineStr"/>
       <c r="J14" s="3" t="inlineStr">
         <is>
           <t>4A</t>
@@ -3166,23 +3230,23 @@
       </c>
       <c r="L14" s="3" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="M14" s="3" t="inlineStr"/>
       <c r="N14" s="3" t="inlineStr">
         <is>
+          <t>4B</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
           <t>5A (1h)</t>
         </is>
       </c>
-      <c r="O14" s="3" t="inlineStr">
-        <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
       <c r="P14" s="3" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>1B (1h)</t>
         </is>
       </c>
     </row>
@@ -3192,38 +3256,42 @@
           <t>MER2</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr"/>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr"/>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>COPERTURA</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>3A (2h)</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>3B (2h)</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>3B (2h)</t>
-        </is>
-      </c>
-      <c r="H15" s="3" t="inlineStr"/>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
           <t>4A</t>
@@ -3236,23 +3304,23 @@
       </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="M15" s="3" t="inlineStr"/>
       <c r="N15" s="3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>4B (2h)</t>
         </is>
       </c>
       <c r="O15" s="3" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="P15" s="3" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
     </row>
@@ -3264,42 +3332,42 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
+          <t>1B (2h)</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>1A (3h)</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>COPERTURA (2h)</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>2A (2h)</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
           <t>COPERTURA (0h 30m)</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>4B (3h)</t>
+          <t>4B (1h)</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
@@ -3308,21 +3376,25 @@
         </is>
       </c>
       <c r="K16" s="3" t="inlineStr"/>
-      <c r="L16" s="3" t="inlineStr"/>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>2B (1h)</t>
+        </is>
+      </c>
       <c r="M16" s="3" t="inlineStr"/>
       <c r="N16" s="3" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="O16" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B (2h)</t>
         </is>
       </c>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -3334,42 +3406,42 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>1A (2h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>5B (3h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>2A (1h)</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B (1h)</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>COPERTURA (2h)</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>COPERTURA</t>
         </is>
       </c>
       <c r="J17" s="3" t="inlineStr">
@@ -3380,15 +3452,19 @@
       <c r="K17" s="3" t="inlineStr"/>
       <c r="L17" s="3" t="inlineStr"/>
       <c r="M17" s="3" t="inlineStr"/>
-      <c r="N17" s="3" t="inlineStr"/>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="O17" s="3" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="P17" s="3" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
     </row>
@@ -3400,42 +3476,42 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>1A (1h 30m)</t>
+          <t>1A (2h 30m)</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>1B (1h 30m)</t>
+          <t>1B (2h 30m)</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2B (3h 30m)</t>
+          <t>2B (1h 30m)</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>2A (3h 30m)</t>
+          <t>2A (1h 30m)</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>3A (1h 30m)</t>
+          <t>3B (2h 30m)</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>3B (1h 30m)</t>
+          <t>3A (3h 30m)</t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>COPERTURA (2h)</t>
         </is>
       </c>
       <c r="J18" s="3" t="inlineStr">
@@ -3446,17 +3522,17 @@
       <c r="K18" s="3" t="inlineStr"/>
       <c r="L18" s="3" t="inlineStr"/>
       <c r="M18" s="3" t="inlineStr"/>
-      <c r="N18" s="3" t="inlineStr"/>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
       <c r="O18" s="3" t="inlineStr">
         <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="P18" s="3" t="inlineStr">
-        <is>
-          <t>COPERTURA (1h)</t>
-        </is>
-      </c>
+          <t>4A (1h)</t>
+        </is>
+      </c>
+      <c r="P18" s="3" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -3468,7 +3544,7 @@
       <c r="C19" s="3" t="inlineStr"/>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
+          <t>5B (3h)</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
@@ -3477,7 +3553,7 @@
       <c r="H19" s="3" t="inlineStr"/>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>4A (3h)</t>
+          <t>4A (1h)</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
@@ -3488,12 +3564,12 @@
       <c r="K19" s="3" t="inlineStr"/>
       <c r="L19" s="3" t="inlineStr"/>
       <c r="M19" s="3" t="inlineStr"/>
-      <c r="N19" s="3" t="inlineStr"/>
-      <c r="O19" s="3" t="inlineStr">
-        <is>
-          <t>5B (2h)</t>
-        </is>
-      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>5A (3h)</t>
+        </is>
+      </c>
+      <c r="O19" s="3" t="inlineStr"/>
       <c r="P19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
@@ -3504,25 +3580,25 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr"/>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
           <t>5B</t>
         </is>
       </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
+      <c r="E20" s="4" t="inlineStr"/>
       <c r="F20" s="4" t="inlineStr"/>
       <c r="G20" s="4" t="inlineStr"/>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -3532,7 +3608,7 @@
       </c>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>4A (1h)</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
@@ -3549,12 +3625,12 @@
       <c r="N20" s="4" t="inlineStr"/>
       <c r="O20" s="4" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
       <c r="P20" s="4" t="inlineStr">
         <is>
-          <t>3A (1h)</t>
+          <t>2A (1h)</t>
         </is>
       </c>
     </row>
@@ -3566,10 +3642,14 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="C21" s="4" t="inlineStr"/>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>1A (2h)</t>
+        </is>
+      </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
           <t>5B</t>
@@ -3577,18 +3657,18 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G21" s="4" t="inlineStr"/>
       <c r="H21" s="4" t="inlineStr">
         <is>
-          <t>3B (2h)</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I21" s="4" t="inlineStr">
@@ -3598,7 +3678,7 @@
       </c>
       <c r="J21" s="4" t="inlineStr">
         <is>
-          <t>4A (2h)</t>
+          <t>BUCO</t>
         </is>
       </c>
       <c r="K21" s="4" t="inlineStr">
@@ -3608,19 +3688,23 @@
       </c>
       <c r="L21" s="4" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>BUCO</t>
         </is>
       </c>
       <c r="M21" s="4" t="inlineStr"/>
-      <c r="N21" s="4" t="inlineStr"/>
+      <c r="N21" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
       <c r="O21" s="4" t="inlineStr">
         <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="P21" s="4" t="inlineStr">
+        <is>
           <t>3A (1h)</t>
-        </is>
-      </c>
-      <c r="P21" s="4" t="inlineStr">
-        <is>
-          <t>2A (1h)</t>
         </is>
       </c>
     </row>
@@ -3632,10 +3716,14 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
+          <t>BUCO (1h)</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr">
+        <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="C22" s="4" t="inlineStr"/>
       <c r="D22" s="4" t="inlineStr">
         <is>
           <t>5B (3h)</t>
@@ -3643,28 +3731,32 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>2A (2h)</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
-        </is>
-      </c>
-      <c r="G22" s="4" t="inlineStr"/>
+          <t>2B (2h)</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>BUCO (2h)</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
@@ -3674,19 +3766,23 @@
       </c>
       <c r="L22" s="4" t="inlineStr">
         <is>
-          <t>1A (2h)</t>
+          <t>BUCO</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr"/>
-      <c r="N22" s="4" t="inlineStr"/>
+      <c r="N22" s="4" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
       <c r="O22" s="4" t="inlineStr">
         <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="P22" s="4" t="inlineStr">
+        <is>
           <t>4B (1h)</t>
-        </is>
-      </c>
-      <c r="P22" s="4" t="inlineStr">
-        <is>
-          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -3698,12 +3794,12 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>1B (3h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>1B (2h)</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
@@ -3713,27 +3809,27 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
-        <is>
-          <t>2B</t>
-        </is>
-      </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A (2h)</t>
         </is>
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
+          <t>3B (3h)</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="J23" s="4" t="inlineStr">
@@ -3746,17 +3842,25 @@
           <t>5B</t>
         </is>
       </c>
-      <c r="L23" s="4" t="inlineStr"/>
+      <c r="L23" s="4" t="inlineStr">
+        <is>
+          <t>BUCO (3h)</t>
+        </is>
+      </c>
       <c r="M23" s="4" t="inlineStr"/>
       <c r="N23" s="4" t="inlineStr">
         <is>
           <t>COPERTURA (1h)</t>
         </is>
       </c>
-      <c r="O23" s="4" t="inlineStr"/>
+      <c r="O23" s="4" t="inlineStr">
+        <is>
+          <t>BUCO</t>
+        </is>
+      </c>
       <c r="P23" s="4" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>2B (1h)</t>
         </is>
       </c>
     </row>
@@ -3768,65 +3872,69 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
+          <t>1B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>COPERTURA (0h 30m)</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>2B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>2A (2h 30m)</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>3B (1h 30m)</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>3A (1h 30m)</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>4B (2h)</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L24" s="4" t="inlineStr">
+        <is>
           <t>1A (1h 30m)</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>1B (1h 30m)</t>
-        </is>
-      </c>
-      <c r="D24" s="4" t="inlineStr">
-        <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>2A (2h 30m)</t>
-        </is>
-      </c>
-      <c r="F24" s="4" t="inlineStr">
-        <is>
-          <t>2B (2h 30m)</t>
-        </is>
-      </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>3A (1h 30m)</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr">
-        <is>
-          <t>3B (1h 30m)</t>
-        </is>
-      </c>
-      <c r="I24" s="4" t="inlineStr">
-        <is>
-          <t>COPERTURA (2h)</t>
-        </is>
-      </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>4B</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>5B</t>
-        </is>
-      </c>
-      <c r="L24" s="4" t="inlineStr"/>
       <c r="M24" s="4" t="inlineStr"/>
-      <c r="N24" s="4" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="O24" s="4" t="inlineStr"/>
+      <c r="N24" s="4" t="inlineStr"/>
+      <c r="O24" s="4" t="inlineStr">
+        <is>
+          <t>BUCO (2h)</t>
+        </is>
+      </c>
       <c r="P24" s="4" t="inlineStr">
         <is>
-          <t>COPERTURA (0h 30m)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
     </row>
@@ -3847,12 +3955,12 @@
       <c r="F25" s="4" t="inlineStr"/>
       <c r="G25" s="4" t="inlineStr"/>
       <c r="H25" s="4" t="inlineStr"/>
-      <c r="I25" s="4" t="inlineStr"/>
-      <c r="J25" s="4" t="inlineStr">
-        <is>
-          <t>4B (3h)</t>
-        </is>
-      </c>
+      <c r="I25" s="4" t="inlineStr">
+        <is>
+          <t>4A (3h)</t>
+        </is>
+      </c>
+      <c r="J25" s="4" t="inlineStr"/>
       <c r="K25" s="4" t="inlineStr">
         <is>
           <t>5B (3h)</t>
@@ -3860,12 +3968,12 @@
       </c>
       <c r="L25" s="4" t="inlineStr"/>
       <c r="M25" s="4" t="inlineStr"/>
-      <c r="N25" s="4" t="inlineStr">
-        <is>
-          <t>4A (2h)</t>
-        </is>
-      </c>
-      <c r="O25" s="4" t="inlineStr"/>
+      <c r="N25" s="4" t="inlineStr"/>
+      <c r="O25" s="4" t="inlineStr">
+        <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
       <c r="P25" s="4" t="inlineStr"/>
     </row>
     <row r="26">
@@ -3874,19 +3982,11 @@
           <t>VEN1</t>
         </is>
       </c>
-      <c r="B26" s="5" t="inlineStr">
-        <is>
-          <t>1B</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
+      <c r="B26" s="5" t="inlineStr"/>
+      <c r="C26" s="5" t="inlineStr"/>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
@@ -3895,38 +3995,46 @@
         </is>
       </c>
       <c r="F26" s="5" t="inlineStr"/>
-      <c r="G26" s="5" t="inlineStr"/>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="J26" s="5" t="inlineStr"/>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="L26" s="5" t="inlineStr">
+        <is>
+          <t>1B (1h)</t>
+        </is>
+      </c>
+      <c r="M26" s="5" t="inlineStr">
+        <is>
           <t>4B (1h)</t>
         </is>
       </c>
-      <c r="J26" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K26" s="5" t="inlineStr"/>
-      <c r="L26" s="5" t="inlineStr"/>
-      <c r="M26" s="5" t="inlineStr">
-        <is>
-          <t>5A (1h)</t>
-        </is>
-      </c>
-      <c r="N26" s="5" t="inlineStr">
-        <is>
-          <t>3B</t>
-        </is>
-      </c>
-      <c r="O26" s="5" t="inlineStr"/>
+      <c r="N26" s="5" t="inlineStr"/>
+      <c r="O26" s="5" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
       <c r="P26" s="5" t="inlineStr">
         <is>
-          <t>2A (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
     </row>
@@ -3938,58 +4046,66 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>1B (2h)</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>1A (2h)</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>5B (2h)</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
+          <t>COPERTURA (1h)</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>3A</t>
+        </is>
+      </c>
+      <c r="H27" s="5" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>4A (2h)</t>
+        </is>
+      </c>
+      <c r="J27" s="5" t="inlineStr"/>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>5A (2h)</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
           <t>2A (1h)</t>
         </is>
       </c>
-      <c r="F27" s="5" t="inlineStr">
-        <is>
-          <t>2B (1h)</t>
-        </is>
-      </c>
-      <c r="G27" s="5" t="inlineStr"/>
-      <c r="H27" s="5" t="inlineStr">
-        <is>
-          <t>3A</t>
-        </is>
-      </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>COPERTURA</t>
-        </is>
-      </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>4A</t>
-        </is>
-      </c>
-      <c r="K27" s="5" t="inlineStr"/>
-      <c r="L27" s="5" t="inlineStr"/>
       <c r="M27" s="5" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
-        </is>
-      </c>
-      <c r="N27" s="5" t="inlineStr">
-        <is>
-          <t>3B (2h)</t>
-        </is>
-      </c>
-      <c r="O27" s="5" t="inlineStr"/>
+          <t>BUCO</t>
+        </is>
+      </c>
+      <c r="N27" s="5" t="inlineStr"/>
+      <c r="O27" s="5" t="inlineStr">
+        <is>
+          <t>BUCO</t>
+        </is>
+      </c>
       <c r="P27" s="5" t="inlineStr">
         <is>
           <t>4B (1h)</t>
@@ -4004,29 +4120,37 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1A (2h)</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
-      <c r="D28" s="5" t="inlineStr"/>
-      <c r="E28" s="5" t="inlineStr"/>
+          <t>1B (2h)</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>5A</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>2A (1h)</t>
+        </is>
+      </c>
       <c r="F28" s="5" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>2B (2h)</t>
         </is>
       </c>
       <c r="G28" s="5" t="inlineStr">
         <is>
-          <t>3B (1h)</t>
+          <t>3A (3h)</t>
         </is>
       </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
-          <t>3A (3h)</t>
+          <t>3B (3h)</t>
         </is>
       </c>
       <c r="I28" s="5" t="inlineStr">
@@ -4036,29 +4160,37 @@
       </c>
       <c r="J28" s="5" t="inlineStr">
         <is>
-          <t>4A (3h)</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="K28" s="5" t="inlineStr">
         <is>
-          <t>5A</t>
-        </is>
-      </c>
-      <c r="L28" s="5" t="inlineStr"/>
-      <c r="M28" s="5" t="inlineStr"/>
+          <t>5B</t>
+        </is>
+      </c>
+      <c r="L28" s="5" t="inlineStr">
+        <is>
+          <t>BUCO</t>
+        </is>
+      </c>
+      <c r="M28" s="5" t="inlineStr">
+        <is>
+          <t>BUCO</t>
+        </is>
+      </c>
       <c r="N28" s="5" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="O28" s="5" t="inlineStr">
         <is>
-          <t>4B (1h)</t>
+          <t>BUCO (2h)</t>
         </is>
       </c>
       <c r="P28" s="5" t="inlineStr">
         <is>
-          <t>2B (1h)</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
     </row>
@@ -4070,11 +4202,19 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>1A (2h)</t>
-        </is>
-      </c>
-      <c r="C29" s="5" t="inlineStr"/>
-      <c r="D29" s="5" t="inlineStr"/>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>1A (1h)</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>5A (2h)</t>
+        </is>
+      </c>
       <c r="E29" s="5" t="inlineStr"/>
       <c r="F29" s="5" t="inlineStr">
         <is>
@@ -4083,38 +4223,42 @@
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>BUCO (1h)</t>
         </is>
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>3A (1h)</t>
         </is>
       </c>
       <c r="I29" s="5" t="inlineStr">
         <is>
-          <t>COPERTURA (3h)</t>
+          <t>COPERTURA (2h)</t>
         </is>
       </c>
       <c r="J29" s="5" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4B (2h)</t>
         </is>
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>5A (2h)</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="L29" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
-        </is>
-      </c>
-      <c r="M29" s="5" t="inlineStr"/>
+          <t>BUCO (2h)</t>
+        </is>
+      </c>
+      <c r="M29" s="5" t="inlineStr">
+        <is>
+          <t>BUCO (3h)</t>
+        </is>
+      </c>
       <c r="N29" s="5" t="inlineStr">
         <is>
-          <t>5B (2h)</t>
+          <t>4A (2h)</t>
         </is>
       </c>
       <c r="O29" s="5" t="inlineStr">
@@ -4124,7 +4268,7 @@
       </c>
       <c r="P29" s="5" t="inlineStr">
         <is>
-          <t>4A (1h)</t>
+          <t>3B (1h)</t>
         </is>
       </c>
     </row>
@@ -4136,7 +4280,7 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>COPERTURA (1h)</t>
+          <t>1B (2h)</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr"/>
@@ -4144,32 +4288,28 @@
       <c r="E30" s="5" t="inlineStr"/>
       <c r="F30" s="5" t="inlineStr">
         <is>
-          <t>2A (3h)</t>
+          <t>2A (2h)</t>
         </is>
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>3A (2h)</t>
-        </is>
-      </c>
-      <c r="H30" s="5" t="inlineStr">
-        <is>
-          <t>3B (2h)</t>
-        </is>
-      </c>
+          <t>3B (1h)</t>
+        </is>
+      </c>
+      <c r="H30" s="5" t="inlineStr"/>
       <c r="I30" s="5" t="inlineStr">
         <is>
+          <t>4B (1h)</t>
+        </is>
+      </c>
+      <c r="J30" s="5" t="inlineStr">
+        <is>
           <t>4A (1h)</t>
         </is>
       </c>
-      <c r="J30" s="5" t="inlineStr">
-        <is>
-          <t>4B (2h)</t>
-        </is>
-      </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>5B (1h)</t>
+          <t>5B (3h)</t>
         </is>
       </c>
       <c r="L30" s="5" t="inlineStr">
@@ -4177,20 +4317,24 @@
           <t>2B (1h)</t>
         </is>
       </c>
-      <c r="M30" s="5" t="inlineStr"/>
+      <c r="M30" s="5" t="inlineStr">
+        <is>
+          <t>5A (1h)</t>
+        </is>
+      </c>
       <c r="N30" s="5" t="inlineStr">
         <is>
-          <t>5A (1h)</t>
+          <t>COPERTURA (1h)</t>
         </is>
       </c>
       <c r="O30" s="5" t="inlineStr">
         <is>
-          <t>1B (1h)</t>
+          <t>1A (1h)</t>
         </is>
       </c>
       <c r="P30" s="5" t="inlineStr">
         <is>
-          <t>1A (1h)</t>
+          <t>3A (1h)</t>
         </is>
       </c>
     </row>

</xml_diff>